<commit_message>
Update R version in App.config (this is copied to the bin directory on each build).
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/AddIn Test.xlsx
+++ b/ExcelRAddIn/Tests/AddIn Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20C6E83-E197-4ED8-B3FD-1870F348DC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F03E8-02C2-4DFB-BA50-B2AE28982CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0F2AA292-504D-47F7-886F-362165F7C2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0F2AA292-504D-47F7-886F-362165F7C2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Model" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>y = rnorm(50)</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>pt &lt;- predict(npk.aov, type = "terms")</t>
+  </si>
+  <si>
+    <t>cf = as.data.frame(summary(fm)$coefficients)</t>
   </si>
 </sst>
 </file>
@@ -666,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC441A8-5743-4B71-A4CB-FCAA901E9088}">
   <dimension ref="B2:BC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,10 +736,10 @@
       </c>
       <c r="E7" cm="1">
         <f t="array" ref="E7:F7">TRANSPOSE(_xll.RScript.Evaluate($B$7&amp;"$"&amp;D7))</f>
-        <v>-0.27764058401493413</v>
+        <v>-8.0426010398750095E-2</v>
       </c>
       <c r="F7">
-        <v>5.3414346465647175E-2</v>
+        <v>0.22845314334593061</v>
       </c>
     </row>
     <row r="8" spans="2:54" x14ac:dyDescent="0.3">
@@ -745,154 +748,154 @@
       </c>
       <c r="E8" cm="1">
         <f t="array" ref="E8:BB8">TRANSPOSE(_xll.RScript.Evaluate($B$7&amp;"$"&amp;D8))</f>
-        <v>-0.12312242970103517</v>
+        <v>2.4153100763592179</v>
       </c>
       <c r="F8">
-        <v>-0.2156566326232088</v>
+        <v>0.15773651600860125</v>
       </c>
       <c r="G8">
-        <v>0.33338367965581622</v>
+        <v>-0.58504401614438628</v>
       </c>
       <c r="H8">
-        <v>-0.69186201059821439</v>
+        <v>-4.3318853568451776E-2</v>
       </c>
       <c r="I8">
-        <v>-0.27296151148917691</v>
+        <v>-0.83619696847580283</v>
       </c>
       <c r="J8">
-        <v>0.16880906718852667</v>
+        <v>-1.6303084891392365</v>
       </c>
       <c r="K8">
-        <v>-1.7376594806863406</v>
+        <v>1.1538848762364673</v>
       </c>
       <c r="L8">
-        <v>0.18750670157578656</v>
+        <v>1.4177660685955087</v>
       </c>
       <c r="M8">
-        <v>-0.5265108537391574</v>
+        <v>0.37079599864830998</v>
       </c>
       <c r="N8">
-        <v>0.12004482498590796</v>
+        <v>1.264129052094904</v>
       </c>
       <c r="O8">
-        <v>1.1734170505829705E-2</v>
+        <v>-6.4121895267565565E-2</v>
       </c>
       <c r="P8">
-        <v>-1.2418633552069667</v>
+        <v>-0.10216784178427801</v>
       </c>
       <c r="Q8">
-        <v>-0.11904022491677083</v>
+        <v>1.0331710612074581</v>
       </c>
       <c r="R8">
-        <v>-2.6529367806763258</v>
+        <v>-0.82615389526715299</v>
       </c>
       <c r="S8">
-        <v>0.463426485047845</v>
+        <v>-0.4247335197918225</v>
       </c>
       <c r="T8">
-        <v>0.72801483278018508</v>
+        <v>-1.2484794917930166</v>
       </c>
       <c r="U8">
-        <v>0.24712957356045967</v>
+        <v>-0.52303575126249535</v>
       </c>
       <c r="V8">
-        <v>-0.45668130112512328</v>
+        <v>-0.14353103893765562</v>
       </c>
       <c r="W8">
-        <v>-0.10588225557306706</v>
+        <v>-4.6272045556871477E-2</v>
       </c>
       <c r="X8">
-        <v>0.45880170585584684</v>
+        <v>0.28189812486014526</v>
       </c>
       <c r="Y8">
-        <v>-0.20401189184580429</v>
+        <v>-1.120171453391144</v>
       </c>
       <c r="Z8">
-        <v>0.38974298761389697</v>
+        <v>1.0110794189761925</v>
       </c>
       <c r="AA8">
-        <v>0.7196499988880517</v>
+        <v>-0.75821712452895329</v>
       </c>
       <c r="AB8">
-        <v>0.18944568991310884</v>
+        <v>-0.48589289326408602</v>
       </c>
       <c r="AC8">
-        <v>2.3939131361540591</v>
+        <v>-0.247916285088848</v>
       </c>
       <c r="AD8">
-        <v>0.48311585562909221</v>
+        <v>-0.56353874026855044</v>
       </c>
       <c r="AE8">
-        <v>-1.5220870997611187</v>
+        <v>-0.45964396089962234</v>
       </c>
       <c r="AF8">
-        <v>0.26761862315115026</v>
+        <v>-4.0393618419368837E-2</v>
       </c>
       <c r="AG8">
-        <v>-1.4147017346397508</v>
+        <v>-0.57090029948597043</v>
       </c>
       <c r="AH8">
-        <v>0.60293089165439395</v>
+        <v>-1.3047264669566796</v>
       </c>
       <c r="AI8">
-        <v>-0.96665321823091188</v>
+        <v>-0.36344902710609017</v>
       </c>
       <c r="AJ8">
-        <v>-0.86521042466076958</v>
+        <v>2.358284604773186</v>
       </c>
       <c r="AK8">
-        <v>-1.2757055490119966</v>
+        <v>-3.1849499652522373E-2</v>
       </c>
       <c r="AL8">
-        <v>-0.25625766357809399</v>
+        <v>-1.2537259636192857</v>
       </c>
       <c r="AM8">
-        <v>-0.84498546934233121</v>
+        <v>0.62695276936630495</v>
       </c>
       <c r="AN8">
-        <v>3.0931548621933276</v>
+        <v>1.0273639469338982</v>
       </c>
       <c r="AO8">
-        <v>1.2735924514438337</v>
+        <v>-2.1608154043195116</v>
       </c>
       <c r="AP8">
-        <v>4.028039450245377E-2</v>
+        <v>1.1115652334964283</v>
       </c>
       <c r="AQ8">
-        <v>5.5547611538063757E-2</v>
+        <v>1.1227540658666095</v>
       </c>
       <c r="AR8">
-        <v>-0.403756756914043</v>
+        <v>0.31062687303533965</v>
       </c>
       <c r="AS8">
-        <v>0.30858045594005451</v>
+        <v>1.1097254493443414</v>
       </c>
       <c r="AT8">
-        <v>1.3782806002480255</v>
+        <v>-0.70105658995467501</v>
       </c>
       <c r="AU8">
-        <v>0.66855828730733502</v>
+        <v>4.5898259812782505E-2</v>
       </c>
       <c r="AV8">
-        <v>2.1333669251412459</v>
+        <v>0.10958903587712238</v>
       </c>
       <c r="AW8">
-        <v>-1.3062882830663007</v>
+        <v>1.0184620357855922</v>
       </c>
       <c r="AX8">
-        <v>-1.1766794975243562</v>
+        <v>-3.0529124193477042</v>
       </c>
       <c r="AY8">
-        <v>-0.93208921889511887</v>
+        <v>0.14315173845186524</v>
       </c>
       <c r="AZ8">
-        <v>-0.45549094233593562</v>
+        <v>2.063408196966543E-2</v>
       </c>
       <c r="BA8">
-        <v>2.5563268268945722</v>
+        <v>1.4047296467661952</v>
       </c>
       <c r="BB8">
-        <v>0.49513794677304923</v>
+        <v>7.3064618825605665E-2</v>
       </c>
     </row>
     <row r="9" spans="2:54" x14ac:dyDescent="0.3">
@@ -901,154 +904,154 @@
       </c>
       <c r="E9" cm="1">
         <f t="array" ref="E9:BB9">TRANSPOSE(_xll.RScript.Evaluate($B$7&amp;"$"&amp;D9))</f>
-        <v>1.9806227215646761</v>
+        <v>0.30616625744381021</v>
       </c>
       <c r="F9">
-        <v>0.36846501822635841</v>
+        <v>1.6323922033574001</v>
       </c>
       <c r="G9">
-        <v>0.36610584189388945</v>
+        <v>-0.91331839658381542</v>
       </c>
       <c r="H9">
-        <v>-0.68778993378755238</v>
+        <v>-0.3331410097912062</v>
       </c>
       <c r="I9">
-        <v>-0.23145010406873173</v>
+        <v>-1.1757385380508438</v>
       </c>
       <c r="J9">
-        <v>0.17997001141524918</v>
+        <v>-1.9239721336927071</v>
       </c>
       <c r="K9">
-        <v>-1.7281488723390661</v>
+        <v>0.89519796969136178</v>
       </c>
       <c r="L9">
-        <v>0.21206307339378211</v>
+        <v>1.107028322348987</v>
       </c>
       <c r="M9">
-        <v>-0.5495440977948115</v>
+        <v>7.6350064565966325E-2</v>
       </c>
       <c r="N9">
-        <v>0.16593761299300963</v>
+        <v>0.98208443442432736</v>
       </c>
       <c r="O9">
-        <v>2.3061411325313246E-2</v>
+        <v>-0.36996100575675561</v>
       </c>
       <c r="P9">
-        <v>-1.2124179994838935</v>
+        <v>-0.40239926100936302</v>
       </c>
       <c r="Q9">
-        <v>-5.6126820473114958E-2</v>
+        <v>0.71249783012182777</v>
       </c>
       <c r="R9">
-        <v>-2.6266522384380422</v>
+        <v>-1.1286834176255633</v>
       </c>
       <c r="S9">
-        <v>0.46729155242512832</v>
+        <v>-0.76019884464142873</v>
       </c>
       <c r="T9">
-        <v>0.73055715648146236</v>
+        <v>-1.5290641309127915</v>
       </c>
       <c r="U9">
-        <v>0.29868099421371236</v>
+        <v>-0.79393136467436787</v>
       </c>
       <c r="V9">
-        <v>-0.45320099261446045</v>
+        <v>-0.45510770549114798</v>
       </c>
       <c r="W9">
-        <v>-0.12463484987374841</v>
+        <v>-0.32291398498191148</v>
       </c>
       <c r="X9">
-        <v>0.47127379996194091</v>
+        <v>-4.1424241693015784E-3</v>
       </c>
       <c r="Y9">
-        <v>-0.20710074484212312</v>
+        <v>-1.4201275052981772</v>
       </c>
       <c r="Z9">
-        <v>0.38725906098269675</v>
+        <v>0.72506193438503985</v>
       </c>
       <c r="AA9">
-        <v>0.72317464554033739</v>
+        <v>-1.0477144905918041</v>
       </c>
       <c r="AB9">
-        <v>0.19947402597883129</v>
+        <v>-0.8215037886619081</v>
       </c>
       <c r="AC9">
-        <v>2.4273196162416313</v>
+        <v>-0.55422670322035361</v>
       </c>
       <c r="AD9">
-        <v>0.54038032615227294</v>
+        <v>-0.87675405045208143</v>
       </c>
       <c r="AE9">
-        <v>-1.5172138309351895</v>
+        <v>-0.77319539210599064</v>
       </c>
       <c r="AF9">
-        <v>0.28997670661442559</v>
+        <v>-0.34431337693121605</v>
       </c>
       <c r="AG9">
-        <v>-1.4577493393709482</v>
+        <v>-0.86169206425562295</v>
       </c>
       <c r="AH9">
-        <v>0.61594697233145068</v>
+        <v>-1.606124813578637</v>
       </c>
       <c r="AI9">
-        <v>-0.98946351178704761</v>
+        <v>-0.66640872458472133</v>
       </c>
       <c r="AJ9">
-        <v>-0.84386018451452427</v>
+        <v>2.0220405146511524</v>
       </c>
       <c r="AK9">
-        <v>-1.2500779786923593</v>
+        <v>-0.3332883809278856</v>
       </c>
       <c r="AL9">
-        <v>-0.22477152866755826</v>
+        <v>-1.535771965181588</v>
       </c>
       <c r="AM9">
-        <v>-0.85384467115421181</v>
+        <v>0.31252962674181028</v>
       </c>
       <c r="AN9">
-        <v>3.114114811817255</v>
+        <v>0.71237806789079028</v>
       </c>
       <c r="AO9">
-        <v>1.309413048594412</v>
+        <v>-2.4814704436689241</v>
       </c>
       <c r="AP9">
-        <v>7.4843776864779929E-2</v>
+        <v>0.80226537342007975</v>
       </c>
       <c r="AQ9">
-        <v>6.6886142467448992E-2</v>
+        <v>0.81597664759979061</v>
       </c>
       <c r="AR9">
-        <v>-0.37073316434855952</v>
+        <v>2.9783979013847106E-3</v>
       </c>
       <c r="AS9">
-        <v>0.3422335834849467</v>
+        <v>0.79281250771755873</v>
       </c>
       <c r="AT9">
-        <v>1.3274030398527077</v>
+        <v>-0.99886020987503887</v>
       </c>
       <c r="AU9">
-        <v>0.63254587281284924</v>
+        <v>-0.23676702676987324</v>
       </c>
       <c r="AV9">
-        <v>2.1583335292004406</v>
+        <v>-0.22405529119387829</v>
       </c>
       <c r="AW9">
-        <v>-1.3013845438906964</v>
+        <v>0.71958542522361457</v>
       </c>
       <c r="AX9">
-        <v>-1.2027217184579506</v>
+        <v>-3.344977451223087</v>
       </c>
       <c r="AY9">
-        <v>-0.85860363990311972</v>
+        <v>-0.15051131878723201</v>
       </c>
       <c r="AZ9">
-        <v>-0.4354932725062301</v>
+        <v>-0.26897942795922103</v>
       </c>
       <c r="BA9">
-        <v>2.5204752838383753</v>
+        <v>1.1145119795348908</v>
       </c>
       <c r="BB9">
-        <v>0.54048269442529928</v>
+        <v>-0.22468235390522726</v>
       </c>
     </row>
     <row r="10" spans="2:54" x14ac:dyDescent="0.3">
@@ -1066,154 +1069,154 @@
       </c>
       <c r="E11" cm="1">
         <f t="array" ref="E11:BB11">TRANSPOSE(_xll.RScript.Evaluate($B$7&amp;"$"&amp;D11))</f>
-        <v>-0.29584726063667838</v>
+        <v>-0.29598683112719115</v>
       </c>
       <c r="F11">
-        <v>-0.30511075763540196</v>
+        <v>-0.28182966919017771</v>
       </c>
       <c r="G11">
-        <v>-0.31617893117486151</v>
+        <v>0.30261478602228542</v>
       </c>
       <c r="H11">
-        <v>-0.26020560854075336</v>
+        <v>-0.19722904943073546</v>
       </c>
       <c r="I11">
-        <v>-0.33335037234035603</v>
+        <v>0.44907796590451887</v>
       </c>
       <c r="J11">
-        <v>-0.27405504239304979</v>
+        <v>-0.14729320566124682</v>
       </c>
       <c r="K11">
-        <v>-0.27083080130416959</v>
+        <v>-0.60195889103804356</v>
       </c>
       <c r="L11">
-        <v>-0.30022552597809321</v>
+        <v>7.4654539912041296E-2</v>
       </c>
       <c r="M11">
-        <v>-0.20725027359785109</v>
+        <v>-0.13712415545641995</v>
       </c>
       <c r="N11">
-        <v>-0.34191022218028372</v>
+        <v>-0.29832995528206452</v>
       </c>
       <c r="O11">
-        <v>-0.27437993401905031</v>
+        <v>1.0976744015642505E-2</v>
       </c>
       <c r="P11">
-        <v>-0.30977707423316603</v>
+        <v>-6.1918126608542151E-2</v>
       </c>
       <c r="Q11">
-        <v>-0.37516319301865853</v>
+        <v>0.20380677883276777</v>
       </c>
       <c r="R11">
-        <v>-0.30360183146055331</v>
+        <v>-3.204488239891834E-2</v>
       </c>
       <c r="S11">
-        <v>-0.25980117673435732</v>
+        <v>0.39609050316828415</v>
       </c>
       <c r="T11">
-        <v>-0.25721694853975413</v>
+        <v>-0.31730834452685475</v>
       </c>
       <c r="U11">
-        <v>-0.35296542379821227</v>
+        <v>-0.44325683958271744</v>
       </c>
       <c r="V11">
-        <v>-0.25904947802713207</v>
+        <v>8.5559738568763546E-2</v>
       </c>
       <c r="W11">
-        <v>-0.21561332683990037</v>
+        <v>-0.36855984369503753</v>
       </c>
       <c r="X11">
-        <v>-0.27661661992850528</v>
+        <v>-0.24638649304253915</v>
       </c>
       <c r="Y11">
-        <v>-0.24621538727380918</v>
+        <v>-6.5497650529910301E-2</v>
       </c>
       <c r="Z11">
-        <v>-0.24739722453884799</v>
+        <v>-0.24668630969903793</v>
       </c>
       <c r="AA11">
-        <v>-0.25913610091390632</v>
+        <v>-0.20145102520849123</v>
       </c>
       <c r="AB11">
-        <v>-0.27184227963622298</v>
+        <v>0.39798278749335092</v>
       </c>
       <c r="AC11">
-        <v>-0.31751587461509345</v>
+        <v>1.7103313399142644E-2</v>
       </c>
       <c r="AD11">
-        <v>-0.36412693968284848</v>
+        <v>0.10686061085026727</v>
       </c>
       <c r="AE11">
-        <v>-0.26177088761386624</v>
+        <v>0.11122987750919244</v>
       </c>
       <c r="AF11">
-        <v>-0.29593075681821379</v>
+        <v>-1.3973080694974445E-2</v>
       </c>
       <c r="AG11">
-        <v>-0.16814846113568782</v>
+        <v>-0.1846250228797981</v>
       </c>
       <c r="AH11">
-        <v>-0.27767939986060231</v>
+        <v>-4.6749135018844923E-2</v>
       </c>
       <c r="AI11">
-        <v>-0.20768584927083078</v>
+        <v>-2.6452998278093609E-2</v>
       </c>
       <c r="AJ11">
-        <v>-0.29396174561607691</v>
+        <v>0.4062137412544442</v>
       </c>
       <c r="AK11">
-        <v>-0.30231831343206017</v>
+        <v>-4.6222221503700034E-2</v>
       </c>
       <c r="AL11">
-        <v>-0.31376411965312556</v>
+        <v>-0.29831196595213605</v>
       </c>
       <c r="AM11">
-        <v>-0.23494192713760442</v>
+        <v>0.12256133069611885</v>
       </c>
       <c r="AN11">
-        <v>-0.29319923978055007</v>
+        <v>0.12987639076244339</v>
       </c>
       <c r="AO11">
-        <v>-0.32223230569124228</v>
+        <v>0.20357030285797384</v>
       </c>
       <c r="AP11">
-        <v>-0.31977610048579896</v>
+        <v>5.596333146089294E-2</v>
       </c>
       <c r="AQ11">
-        <v>-0.27440199136913057</v>
+        <v>2.3173889121284708E-2</v>
       </c>
       <c r="AR11">
-        <v>-0.31676783193086744</v>
+        <v>3.4496833742473143E-2</v>
       </c>
       <c r="AS11">
-        <v>-0.31799774674564807</v>
+        <v>0.15492644632111063</v>
       </c>
       <c r="AT11">
-        <v>-0.15285117220756295</v>
+        <v>-9.3477302726518663E-2</v>
       </c>
       <c r="AU11">
-        <v>-0.18189302653705386</v>
+        <v>-0.29026182565159531</v>
       </c>
       <c r="AV11">
-        <v>-0.30102699170669434</v>
+        <v>0.37241919331425094</v>
       </c>
       <c r="AW11">
-        <v>-0.26183041716457089</v>
+        <v>-7.9529403258147613E-2</v>
       </c>
       <c r="AX11">
-        <v>-0.20137167215304053</v>
+        <v>-0.1680737120870055</v>
       </c>
       <c r="AY11">
-        <v>-0.39581792155124251</v>
+        <v>-0.1473008402123033</v>
       </c>
       <c r="AZ11">
-        <v>-0.29131924547747129</v>
+        <v>-0.19994126090626302</v>
       </c>
       <c r="BA11">
-        <v>-0.18220731910489851</v>
+        <v>-0.19208776713810516</v>
       </c>
       <c r="BB11">
-        <v>-0.34083952242002158</v>
+        <v>-9.4213664512075565E-2</v>
       </c>
     </row>
     <row r="12" spans="2:54" x14ac:dyDescent="0.3">
@@ -1449,154 +1452,154 @@
         <v>y</v>
       </c>
       <c r="F19">
-        <v>-0.41896969033771353</v>
+        <v>2.1193232452320268</v>
       </c>
       <c r="G19">
-        <v>-0.52076739025861074</v>
+        <v>-0.12409315318157643</v>
       </c>
       <c r="H19">
-        <v>1.7204748480954712E-2</v>
+        <v>-0.28242923012210086</v>
       </c>
       <c r="I19">
-        <v>-0.95206761913896776</v>
+        <v>-0.24054790299918724</v>
       </c>
       <c r="J19">
-        <v>-0.60631188382953294</v>
+        <v>-0.38711900257128395</v>
       </c>
       <c r="K19">
-        <v>-0.10524597520452308</v>
+        <v>-1.7776016948004834</v>
       </c>
       <c r="L19">
-        <v>-2.0084902819905102</v>
+        <v>0.55192598519842373</v>
       </c>
       <c r="M19">
-        <v>-0.11271882440230667</v>
+        <v>1.49242060850755</v>
       </c>
       <c r="N19">
-        <v>-0.73376112733700849</v>
+        <v>0.23367184319189002</v>
       </c>
       <c r="O19">
-        <v>-0.22186539719437576</v>
+        <v>0.96579909681283949</v>
       </c>
       <c r="P19">
-        <v>-0.26264576351322061</v>
+        <v>-5.314515125192306E-2</v>
       </c>
       <c r="Q19">
-        <v>-1.5516404294401327</v>
+        <v>-0.16408596839282016</v>
       </c>
       <c r="R19">
-        <v>-0.49420341793542932</v>
+        <v>1.2369778400402258</v>
       </c>
       <c r="S19">
-        <v>-2.9565386121368791</v>
+        <v>-0.85819877766607133</v>
       </c>
       <c r="T19">
-        <v>0.20362530831348769</v>
+        <v>-2.8643016623538371E-2</v>
       </c>
       <c r="U19">
-        <v>0.47079788424043095</v>
+        <v>-1.5657878363198714</v>
       </c>
       <c r="V19">
-        <v>-0.10583585023775262</v>
+        <v>-0.9662925908452128</v>
       </c>
       <c r="W19">
-        <v>-0.71573077915225536</v>
+        <v>-5.7971300368892073E-2</v>
       </c>
       <c r="X19">
-        <v>-0.32149558241296744</v>
+        <v>-0.414831889251909</v>
       </c>
       <c r="Y19">
-        <v>0.18218508592734156</v>
+        <v>3.551163181760611E-2</v>
       </c>
       <c r="Z19">
-        <v>-0.45022727911961347</v>
+        <v>-1.1856691039210543</v>
       </c>
       <c r="AA19">
-        <v>0.14234576307504898</v>
+        <v>0.76439310927715454</v>
       </c>
       <c r="AB19">
-        <v>0.46051389797414538</v>
+        <v>-0.95966814973744452</v>
       </c>
       <c r="AC19">
-        <v>-8.2396589723114172E-2</v>
+        <v>-8.7910105770735089E-2</v>
       </c>
       <c r="AD19">
-        <v>2.0763972615389656</v>
+        <v>-0.23081297168970535</v>
       </c>
       <c r="AE19">
-        <v>0.11898891594624371</v>
+        <v>-0.45667812941828317</v>
       </c>
       <c r="AF19">
-        <v>-1.7838579873749849</v>
+        <v>-0.3484140833904299</v>
       </c>
       <c r="AG19">
-        <v>-2.8312133667063515E-2</v>
+        <v>-5.4366699114343282E-2</v>
       </c>
       <c r="AH19">
-        <v>-1.5828501957754386</v>
+        <v>-0.75552532236576853</v>
       </c>
       <c r="AI19">
-        <v>0.32525149179379165</v>
+        <v>-1.3514756019755245</v>
       </c>
       <c r="AJ19">
-        <v>-1.1743390675017427</v>
+        <v>-0.38990202538418378</v>
       </c>
       <c r="AK19">
-        <v>-1.1591721702768465</v>
+        <v>2.7644983460276302</v>
       </c>
       <c r="AL19">
-        <v>-1.5780238624440568</v>
+        <v>-7.8071721156222407E-2</v>
       </c>
       <c r="AM19">
-        <v>-0.57002178323121955</v>
+        <v>-1.5520379295714217</v>
       </c>
       <c r="AN19">
-        <v>-1.0799273964799356</v>
+        <v>0.7495141000624238</v>
       </c>
       <c r="AO19">
-        <v>2.7999556224127775</v>
+        <v>1.1572403376963416</v>
       </c>
       <c r="AP19">
-        <v>0.95136014575259142</v>
+        <v>-1.9572451014615377</v>
       </c>
       <c r="AQ19">
-        <v>-0.27949570598334522</v>
+        <v>1.1675285649573213</v>
       </c>
       <c r="AR19">
-        <v>-0.21885437983106681</v>
+        <v>1.1459279549878942</v>
       </c>
       <c r="AS19">
-        <v>-0.72052458884491044</v>
+        <v>0.34512370677781279</v>
       </c>
       <c r="AT19">
-        <v>-9.4172908055935502E-3</v>
+        <v>1.264651895665452</v>
       </c>
       <c r="AU19">
-        <v>1.2254294280404625</v>
+        <v>-0.79453389268119368</v>
       </c>
       <c r="AV19">
-        <v>0.48666526077028116</v>
+        <v>-0.24436356583881277</v>
       </c>
       <c r="AW19">
-        <v>1.8323399334345516</v>
+        <v>0.48200822919137332</v>
       </c>
       <c r="AX19">
-        <v>-1.5681187002308716</v>
+        <v>0.93893263252744463</v>
       </c>
       <c r="AY19">
-        <v>-1.3780511696773967</v>
+        <v>-3.2209861314347097</v>
       </c>
       <c r="AZ19">
-        <v>-1.3279071404463614</v>
+        <v>-4.1491017604380672E-3</v>
       </c>
       <c r="BA19">
-        <v>-0.74681018781340691</v>
+        <v>-0.17930717893659759</v>
       </c>
       <c r="BB19">
-        <v>2.3741195077896737</v>
+        <v>1.21264187962809</v>
       </c>
       <c r="BC19">
-        <v>0.15429842435302762</v>
+        <v>-2.1149045686469903E-2</v>
       </c>
     </row>
     <row r="20" spans="2:55" x14ac:dyDescent="0.3">
@@ -1604,154 +1607,154 @@
         <v>x</v>
       </c>
       <c r="F20">
-        <v>-0.34085742551307985</v>
+        <v>-0.94356688453191018</v>
       </c>
       <c r="G20">
-        <v>-0.51428455907694137</v>
+        <v>-0.88159723189475303</v>
       </c>
       <c r="H20">
-        <v>-0.7214980564203447</v>
+        <v>1.6766711580808655</v>
       </c>
       <c r="I20">
-        <v>0.32640997461971855</v>
+        <v>-0.51127788097500071</v>
       </c>
       <c r="J20">
-        <v>-1.0429742571361613</v>
+        <v>2.3177793421799326</v>
       </c>
       <c r="K20">
-        <v>6.7126939841722952E-2</v>
+        <v>-0.29269544854213025</v>
       </c>
       <c r="L20">
-        <v>0.12748976934772191</v>
+        <v>-2.2828877423217278</v>
       </c>
       <c r="M20">
-        <v>-0.4228253916330198</v>
+        <v>0.67882870001032913</v>
       </c>
       <c r="N20">
-        <v>1.3178165619297428</v>
+        <v>-0.24818281870526029</v>
       </c>
       <c r="O20">
-        <v>-1.203228016777925</v>
+        <v>-0.95382336041381577</v>
       </c>
       <c r="P20">
-        <v>6.1044461116470529E-2</v>
+        <v>0.40009409840331134</v>
       </c>
       <c r="Q20">
-        <v>-0.6016452946569314</v>
+        <v>8.1013916110502723E-2</v>
       </c>
       <c r="R20">
-        <v>-1.8257755726066021</v>
+        <v>1.2441623042197505</v>
       </c>
       <c r="S20">
-        <v>-0.48603510411413048</v>
+        <v>0.21177702915897986</v>
       </c>
       <c r="T20">
-        <v>0.33398156976515753</v>
+        <v>2.0858391641627736</v>
       </c>
       <c r="U20">
-        <v>0.38236235817872261</v>
+        <v>-1.0368968036890187</v>
       </c>
       <c r="V20">
-        <v>-1.4101986594879055</v>
+        <v>-1.5882067712877039</v>
       </c>
       <c r="W20">
-        <v>0.34805454373122063</v>
+        <v>0.72656364686640773</v>
       </c>
       <c r="X20">
-        <v>1.1612471420000621</v>
+        <v>-1.2612382087471941</v>
       </c>
       <c r="Y20">
-        <v>1.917020714813927E-2</v>
+        <v>-0.72645304946619516</v>
       </c>
       <c r="Z20">
-        <v>0.58832876971238091</v>
+        <v>6.5345390526033248E-2</v>
       </c>
       <c r="AA20">
-        <v>0.5662029300599396</v>
+        <v>-0.72776542649068088</v>
       </c>
       <c r="AB20">
-        <v>0.34643282798430974</v>
+        <v>-0.52975858872942505</v>
       </c>
       <c r="AC20">
-        <v>0.10855331502446262</v>
+        <v>2.0941221945354456</v>
       </c>
       <c r="AD20">
-        <v>-0.74652772595102401</v>
+        <v>0.4269117175166674</v>
       </c>
       <c r="AE20">
-        <v>-1.6191596713354355</v>
+        <v>0.81980321437478476</v>
       </c>
       <c r="AF20">
-        <v>0.29710550537718255</v>
+        <v>0.83892865338136913</v>
       </c>
       <c r="AG20">
-        <v>-0.34242060445395034</v>
+        <v>0.29088209831786183</v>
       </c>
       <c r="AH20">
-        <v>2.0498635689508102</v>
+        <v>-0.45610671385364471</v>
       </c>
       <c r="AI20">
-        <v>-7.2669326194927319E-4</v>
+        <v>0.14741261550037305</v>
       </c>
       <c r="AJ20">
-        <v>1.3096619049545815</v>
+        <v>0.23625418906549672</v>
       </c>
       <c r="AK20">
-        <v>-0.30555763911928496</v>
+        <v>2.1301512622057008</v>
       </c>
       <c r="AL20">
-        <v>-0.46200564174265929</v>
+        <v>0.14971905570700567</v>
       </c>
       <c r="AM20">
-        <v>-0.67628901275472619</v>
+        <v>-0.95374461634549068</v>
       </c>
       <c r="AN20">
-        <v>0.79938555280819545</v>
+        <v>0.88852942936967749</v>
       </c>
       <c r="AO20">
-        <v>-0.29128233883049814</v>
+        <v>0.92054938741966508</v>
       </c>
       <c r="AP20">
-        <v>-0.83482668284609485</v>
+        <v>1.2431271861586424</v>
       </c>
       <c r="AQ20">
-        <v>-0.78884268476379904</v>
+        <v>0.59701232323653386</v>
       </c>
       <c r="AR20">
-        <v>6.0631513068993247E-2</v>
+        <v>0.4534842375233179</v>
       </c>
       <c r="AS20">
-        <v>-0.73252319844627434</v>
+        <v>0.503047769262704</v>
       </c>
       <c r="AT20">
-        <v>-0.75554912492787185</v>
+        <v>1.0302001245107968</v>
       </c>
       <c r="AU20">
-        <v>2.3362527123238022</v>
+        <v>-5.7128968052788533E-2</v>
       </c>
       <c r="AV20">
-        <v>1.7925438353806176</v>
+        <v>-0.91850701714839411</v>
       </c>
       <c r="AW20">
-        <v>-0.4378300819762127</v>
+        <v>1.9822235626991971</v>
       </c>
       <c r="AX20">
-        <v>0.29599101920176862</v>
+        <v>3.9246872573981276E-3</v>
       </c>
       <c r="AY20">
-        <v>1.4278731634570361</v>
+        <v>-0.38365723668567181</v>
       </c>
       <c r="AZ20">
-        <v>-2.2124643537914084</v>
+        <v>-0.29272886699698158</v>
       </c>
       <c r="BA20">
-        <v>-0.25608590889218036</v>
+        <v>-0.5231499499507406</v>
       </c>
       <c r="BB20">
-        <v>1.7866597875799615</v>
+        <v>-0.48877312478153806</v>
       </c>
       <c r="BC20">
-        <v>-1.1831828448136708</v>
+        <v>-6.0352218890014846E-2</v>
       </c>
     </row>
     <row r="22" spans="2:55" x14ac:dyDescent="0.3">
@@ -1975,16 +1978,19 @@
       </c>
       <c r="J27" cm="1">
         <f t="array" ref="J27:M28">_xll.RScript.Evaluate($B$22&amp;"$"&amp;D25)</f>
-        <v>-0.27764058401493413</v>
+        <v>-8.0426010398750095E-2</v>
       </c>
       <c r="K27">
-        <v>0.15667804436530869</v>
+        <v>0.15234254400271344</v>
       </c>
       <c r="L27">
-        <v>-1.7720452482007665</v>
+        <v>-0.52792876031607816</v>
       </c>
       <c r="M27">
-        <v>8.273436771475863E-2</v>
+        <v>0.59998100273017685</v>
+      </c>
+      <c r="P27" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:55" x14ac:dyDescent="0.3">
@@ -2005,16 +2011,16 @@
         <v>10</v>
       </c>
       <c r="J28">
-        <v>5.3414346465647175E-2</v>
+        <v>0.22845314334593061</v>
       </c>
       <c r="K28">
-        <v>0.16042449965622421</v>
+        <v>0.14884481412361331</v>
       </c>
       <c r="L28">
-        <v>0.33295629146489147</v>
+        <v>1.5348411343119004</v>
       </c>
       <c r="M28">
-        <v>0.7406172160162855</v>
+        <v>0.13138863174563695</v>
       </c>
     </row>
     <row r="29" spans="2:55" x14ac:dyDescent="0.3">
@@ -2025,6 +2031,26 @@
         <f t="array" ref="E29">TRANSPOSE(_xll.RScript.Evaluate($B$22&amp;"$"&amp;D29))</f>
         <v>2.3042592103914468E-3</v>
       </c>
+      <c r="P29" t="str" cm="1">
+        <f t="array" ref="P29">_xll.RScript.Evaluate(P27)</f>
+        <v>cf</v>
+      </c>
+      <c r="Q29" t="str" cm="1">
+        <f t="array" ref="Q29:U31">_xll.RScript.Evaluate(P29)</f>
+        <v>Index</v>
+      </c>
+      <c r="R29" t="str">
+        <v>Estimate</v>
+      </c>
+      <c r="S29" t="str">
+        <v>Std. Error</v>
+      </c>
+      <c r="T29" t="str">
+        <v>t value</v>
+      </c>
+      <c r="U29" t="str">
+        <v>Pr(&gt;|t|)</v>
+      </c>
     </row>
     <row r="30" spans="2:55" x14ac:dyDescent="0.3">
       <c r="D30" t="str">
@@ -2034,6 +2060,21 @@
         <f t="array" ref="E30">TRANSPOSE(_xll.RScript.Evaluate($B$22&amp;"$"&amp;D30))</f>
         <v>-1.8481068722725258E-2</v>
       </c>
+      <c r="Q30" t="str">
+        <v>(Intercept)</v>
+      </c>
+      <c r="R30">
+        <v>-8.0426010398750095E-2</v>
+      </c>
+      <c r="S30">
+        <v>0.15234254400271344</v>
+      </c>
+      <c r="T30">
+        <v>-0.52792876031607816</v>
+      </c>
+      <c r="U30">
+        <v>0.59998100273017685</v>
+      </c>
     </row>
     <row r="31" spans="2:55" x14ac:dyDescent="0.3">
       <c r="D31" t="str">
@@ -2048,6 +2089,21 @@
       </c>
       <c r="G31">
         <v>48</v>
+      </c>
+      <c r="Q31" t="str">
+        <v>x</v>
+      </c>
+      <c r="R31">
+        <v>0.22845314334593061</v>
+      </c>
+      <c r="S31">
+        <v>0.14884481412361331</v>
+      </c>
+      <c r="T31">
+        <v>1.5348411343119004</v>
+      </c>
+      <c r="U31">
+        <v>0.13138863174563695</v>
       </c>
     </row>
     <row r="32" spans="2:55" x14ac:dyDescent="0.3">
@@ -2153,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E54137A-AC86-4C17-97C8-77A96C22EEAE}">
   <dimension ref="B2:Q57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated REnvironmentControlLibrary with new icons, improved colour scheme. Updated the RibbonController to use the new Office365 icons.
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/AddIn Test.xlsx
+++ b/ExcelRAddIn/Tests/AddIn Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BE9704-55C6-4819-971B-B4B12A10C051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9F1BB9-9693-44C7-9B0B-4C5B85D50B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0F2AA292-504D-47F7-886F-362165F7C2B7}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{0F2AA292-504D-47F7-886F-362165F7C2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Model" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -205,7 +205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -292,13 +292,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,9 +496,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -536,7 +536,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -642,7 +642,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -784,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC441A8-5743-4B71-A4CB-FCAA901E9088}">
   <dimension ref="B2:BC111"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2538,254 +2538,254 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="5.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="str">
+      <c r="B3" s="8" t="str">
         <f>"Call: "&amp;'Linear Model'!E34</f>
         <v>Call: lm(formula = y ~ x)</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="str" cm="1">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="str" cm="1">
         <f t="array" ref="D5:I6">TRANSPOSE('Linear Model'!E48:F53)</f>
         <v>Min.</v>
       </c>
-      <c r="E5" s="9" t="str">
+      <c r="E5" s="8" t="str">
         <v>1st Qu.</v>
       </c>
-      <c r="F5" s="9" t="str">
+      <c r="F5" s="8" t="str">
         <v>Median</v>
       </c>
-      <c r="G5" s="9" t="str">
+      <c r="G5" s="8" t="str">
         <v>Mean</v>
       </c>
-      <c r="H5" s="9" t="str">
+      <c r="H5" s="8" t="str">
         <v>3rd Qu.</v>
       </c>
-      <c r="I5" s="9" t="str">
+      <c r="I5" s="8" t="str">
         <v>Max.</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>-2.1263388022976604</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>-0.49439097369794727</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>7.7320990562112002E-2</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>2.1103995287430344E-17</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>0.60608140860427218</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>2.3182085031953807</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="str" cm="1">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="str" cm="1">
         <f t="array" ref="D8:H10">_xlfn.ANCHORARRAY('Linear Model'!E55)</f>
         <v>Index</v>
       </c>
-      <c r="E8" s="9" t="str">
+      <c r="E8" s="8" t="str">
         <v>Estimate</v>
       </c>
-      <c r="F8" s="9" t="str">
+      <c r="F8" s="8" t="str">
         <v>Std. Error</v>
       </c>
-      <c r="G8" s="9" t="str">
+      <c r="G8" s="8" t="str">
         <v>t value</v>
       </c>
-      <c r="H8" s="9" t="str">
+      <c r="H8" s="8" t="str">
         <v>Pr(&gt;|t|)</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D9" s="9" t="str">
+      <c r="D9" s="8" t="str">
         <v>(Intercept)</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>7.85E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>0.1404</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>0.55940000000000001</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>0.57850000000000001</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D10" s="9" t="str">
+      <c r="D10" s="8" t="str">
         <v>x</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>9.6100000000000005E-2</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>0.13200000000000001</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>0.72819999999999996</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>0.47</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="str">
+      <c r="B12" s="8" t="str">
         <f>"Residual standard error: "&amp;ROUND('Linear Model'!E39, 3)&amp;" on "&amp;'Linear Model'!E26&amp;" degrees of freedom"</f>
         <v>Residual standard error: 0.977 on 48 degrees of freedom</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="str">
+      <c r="B13" s="8" t="str">
         <f>"Multiple R-squared: "&amp;ROUND('Linear Model'!E41, 4)</f>
         <v>Multiple R-squared: 0.0109</v>
       </c>
-      <c r="C13" s="9" t="str">
+      <c r="C13" s="8" t="str">
         <f>"Adjusted R-squared: "&amp;ROUND('Linear Model'!E42, 4)</f>
         <v>Adjusted R-squared: -0.0097</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="str">
+      <c r="B14" s="8" t="str">
         <f>"F-statistic: "&amp;ROUND('Linear Model'!E43, 2)&amp;" on "&amp;'Linear Model'!F43&amp;" and "&amp;'Linear Model'!G43&amp;" DF"</f>
         <v>F-statistic: 0.53 on 1 and 48 DF</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="str" cm="1">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="str" cm="1">
         <f t="array" ref="D16:I18">_xlfn.ANCHORARRAY('Linear Model'!E59)</f>
         <v>Index</v>
       </c>
-      <c r="E16" s="9" t="str">
+      <c r="E16" s="8" t="str">
         <v>Df</v>
       </c>
-      <c r="F16" s="9" t="str">
+      <c r="F16" s="8" t="str">
         <v>Sum Sq</v>
       </c>
-      <c r="G16" s="9" t="str">
+      <c r="G16" s="8" t="str">
         <v>Mean Sq</v>
       </c>
-      <c r="H16" s="9" t="str">
+      <c r="H16" s="8" t="str">
         <v>F value</v>
       </c>
-      <c r="I16" s="9" t="str">
+      <c r="I16" s="8" t="str">
         <v>Pr(&gt;F)</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9" t="str">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="str">
         <v>x</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>1</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>0.26452252628379735</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="10">
         <v>0.26452252628379735</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>0.3670113113185195</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>0.54749204609353308</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9" t="str">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="str">
         <v>Residuals</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>48</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>34.595885385676326</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>0.72074761220159012</v>
       </c>
-      <c r="H18" s="9" t="str">
+      <c r="H18" s="8" t="str">
         <v/>
       </c>
-      <c r="I18" s="9" t="str">
+      <c r="I18" s="8" t="str">
         <v/>
       </c>
     </row>
@@ -2802,7 +2802,7 @@
   <dimension ref="B2:Q57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Rebuild and publish the ExcelRAddIn and the RScriptAddIn.
</commit_message>
<xml_diff>
--- a/ExcelRAddIn/Tests/AddIn Test.xlsx
+++ b/ExcelRAddIn/Tests/AddIn Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\C#\Office\Office365 AddIns\ExcelRAddIn\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9F1BB9-9693-44C7-9B0B-4C5B85D50B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C856FB5A-FD87-4CCB-A534-0267907691FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{0F2AA292-504D-47F7-886F-362165F7C2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0F2AA292-504D-47F7-886F-362165F7C2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Model" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC441A8-5743-4B71-A4CB-FCAA901E9088}">
   <dimension ref="B2:BC111"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,10 +869,10 @@
       </c>
       <c r="E19" s="5" cm="1">
         <f t="array" ref="E19:F19">TRANSPOSE(_xll.RScript.Evaluate($B$19&amp;"$"&amp;D19))</f>
-        <v>7.8534553462568338E-2</v>
+        <v>-0.10992862344108487</v>
       </c>
       <c r="F19" s="5">
-        <v>9.6124662652678439E-2</v>
+        <v>-0.12593349412011373</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -892,154 +892,154 @@
       </c>
       <c r="E20" s="5" cm="1">
         <f t="array" ref="E20:BB20">TRANSPOSE(_xll.RScript.Evaluate($B$19&amp;"$"&amp;D20))</f>
-        <v>0.14544475288926215</v>
+        <v>-1.8721562686739972</v>
       </c>
       <c r="F20" s="5">
-        <v>1.6982297065551539</v>
+        <v>-1.5318705646200841</v>
       </c>
       <c r="G20" s="5">
-        <v>-0.32826482498224052</v>
+        <v>5.551462165872828E-2</v>
       </c>
       <c r="H20" s="5">
-        <v>-2.1263388022976604</v>
+        <v>0.73316980344449134</v>
       </c>
       <c r="I20" s="5">
-        <v>-0.87651741598721566</v>
+        <v>-0.16768496711630598</v>
       </c>
       <c r="J20" s="5">
-        <v>0.26318630558144473</v>
+        <v>-0.17073380696018381</v>
       </c>
       <c r="K20" s="5">
-        <v>2.3182085031953807</v>
+        <v>-0.24030190204656127</v>
       </c>
       <c r="L20" s="5">
-        <v>0.88751133590512266</v>
+        <v>1.3493555798811001</v>
       </c>
       <c r="M20" s="5">
-        <v>0.60408830355245069</v>
+        <v>2.3786028457893273</v>
       </c>
       <c r="N20" s="5">
-        <v>-1.8503657907532607</v>
+        <v>0.37558627322264182</v>
       </c>
       <c r="O20" s="5">
-        <v>-0.64774056473127894</v>
+        <v>0.94543301648422462</v>
       </c>
       <c r="P20" s="5">
-        <v>-0.32899910093210705</v>
+        <v>-4.591878006104419E-2</v>
       </c>
       <c r="Q20" s="5">
-        <v>-7.2617769708340385E-2</v>
+        <v>-0.51149597908336286</v>
       </c>
       <c r="R20">
-        <v>0.41557834837444713</v>
+        <v>0.47776781166117355</v>
       </c>
       <c r="S20">
-        <v>-0.69404440468102579</v>
+        <v>-7.4027806888877029E-2</v>
       </c>
       <c r="T20">
-        <v>0.87292246234179305</v>
+        <v>-1.7428818212718473</v>
       </c>
       <c r="U20">
-        <v>0.17606659375262068</v>
+        <v>-1.4843698844308046</v>
       </c>
       <c r="V20">
-        <v>0.14704321192089187</v>
+        <v>-0.56623052476683311</v>
       </c>
       <c r="W20">
-        <v>-0.58658013906890016</v>
+        <v>0.3384404510038026</v>
       </c>
       <c r="X20">
-        <v>-0.20332186483209674</v>
+        <v>0.3155645217983315</v>
       </c>
       <c r="Y20">
-        <v>-0.96859311945873572</v>
+        <v>1.2222105664736784</v>
       </c>
       <c r="Z20">
-        <v>0.46436704683775254</v>
+        <v>0.44867150317028426</v>
       </c>
       <c r="AA20">
-        <v>0.87644553418109372</v>
+        <v>0.12889912685808491</v>
       </c>
       <c r="AB20">
-        <v>0.83831405512318524</v>
+        <v>0.35830665626635749</v>
       </c>
       <c r="AC20">
-        <v>-0.44561099332094889</v>
+        <v>0.23474176303264821</v>
       </c>
       <c r="AD20">
-        <v>-0.67254861386887654</v>
+        <v>-0.84941988768043453</v>
       </c>
       <c r="AE20">
-        <v>-0.22146361163709904</v>
+        <v>-0.40438163701960839</v>
       </c>
       <c r="AF20">
-        <v>0.85768863450376076</v>
+        <v>2.1149915797974539E-2</v>
       </c>
       <c r="AG20">
-        <v>-0.48829184760834998</v>
+        <v>-0.93272125686417617</v>
       </c>
       <c r="AH20">
-        <v>4.4391245049364758E-2</v>
+        <v>0.97970028651819141</v>
       </c>
       <c r="AI20">
-        <v>0.1971529390979154</v>
+        <v>8.4179586496066494E-3</v>
       </c>
       <c r="AJ20">
-        <v>0.6067457769548793</v>
+        <v>0.1427396270291843</v>
       </c>
       <c r="AK20">
-        <v>-2.0336075302121368</v>
+        <v>-0.98436881392814657</v>
       </c>
       <c r="AL20">
-        <v>0.12931593861011187</v>
+        <v>0.55186624731696843</v>
       </c>
       <c r="AM20">
-        <v>-0.43457594147347955</v>
+        <v>1.9634999263347441</v>
       </c>
       <c r="AN20">
-        <v>-0.9053138934939321</v>
+        <v>-0.99619166616374577</v>
       </c>
       <c r="AO20">
-        <v>-0.38687570965990892</v>
+        <v>0.77937932680732036</v>
       </c>
       <c r="AP20">
-        <v>-1.4643899612306777</v>
+        <v>0.94853880316701211</v>
       </c>
       <c r="AQ20">
-        <v>0.42431191702343007</v>
+        <v>-1.1826772220546946</v>
       </c>
       <c r="AR20">
-        <v>-0.46362526515927061</v>
+        <v>-0.32374288421780917</v>
       </c>
       <c r="AS20">
-        <v>0.11025073607485925</v>
+        <v>-0.64694522895365747</v>
       </c>
       <c r="AT20">
-        <v>0.84893983710431065</v>
+        <v>-1.479295260502365</v>
       </c>
       <c r="AU20">
-        <v>-1.6706344201214827</v>
+        <v>-7.8072420766197803E-2</v>
       </c>
       <c r="AV20">
-        <v>0.59090941579041489</v>
+        <v>0.60280971997060473</v>
       </c>
       <c r="AW20">
-        <v>1.0954397281243871</v>
+        <v>-0.99239026607380909</v>
       </c>
       <c r="AX20">
-        <v>-0.49642401572781303</v>
+        <v>0.65475626088226946</v>
       </c>
       <c r="AY20">
-        <v>0.65426510278509531</v>
+        <v>1.1586191109961788</v>
       </c>
       <c r="AZ20">
-        <v>1.2512922596446669</v>
+        <v>-0.84794250701683793</v>
       </c>
       <c r="BA20">
-        <v>2.2548640784614786</v>
+        <v>-0.58747913560608056</v>
       </c>
       <c r="BB20">
-        <v>-0.40622816848843513</v>
+        <v>1.5395587685525369</v>
       </c>
     </row>
     <row r="21" spans="2:55" x14ac:dyDescent="0.3">
@@ -1048,154 +1048,154 @@
       </c>
       <c r="E21" s="5" cm="1">
         <f t="array" ref="E21:BB21">TRANSPOSE(_xll.RScript.Evaluate($B$19&amp;"$"&amp;D21))</f>
-        <v>-0.6827468611324834</v>
+        <v>0.42288766791490029</v>
       </c>
       <c r="F21" s="5">
-        <v>-0.71156110085390267</v>
+        <v>1.0077316688784892</v>
       </c>
       <c r="G21" s="5">
-        <v>-0.23486717465009313</v>
+        <v>3.3628163933942135E-2</v>
       </c>
       <c r="H21" s="5">
-        <v>-1.841353000609091</v>
+        <v>0.93263550827948105</v>
       </c>
       <c r="I21" s="5">
-        <v>-0.94806560779494964</v>
+        <v>2.18558934908889E-2</v>
       </c>
       <c r="J21" s="5">
-        <v>0.5056090314138314</v>
+        <v>0.23054411661087337</v>
       </c>
       <c r="K21" s="5">
-        <v>2.1918852482433597</v>
+        <v>-0.43699863532665117</v>
       </c>
       <c r="L21" s="5">
-        <v>1.0088723016391516</v>
+        <v>1.51641981029971</v>
       </c>
       <c r="M21" s="5">
-        <v>0.62232895708882741</v>
+        <v>2.7643385118866779</v>
       </c>
       <c r="N21" s="5">
-        <v>-2.0501698015596634</v>
+        <v>0.79545729445241797</v>
       </c>
       <c r="O21" s="5">
-        <v>-0.3904448589628417</v>
+        <v>0.91072967324997833</v>
       </c>
       <c r="P21" s="5">
-        <v>-0.11671821732861376</v>
+        <v>0.11285909428176194</v>
       </c>
       <c r="Q21" s="5">
-        <v>-0.48539339439008333</v>
+        <v>-0.25410123990468997</v>
       </c>
       <c r="R21">
-        <v>0.21956368107900276</v>
+        <v>0.74824886339006336</v>
       </c>
       <c r="S21">
-        <v>-0.69610552679029991</v>
+        <v>-4.1399397622763845E-2</v>
       </c>
       <c r="T21">
-        <v>0.65172711225956159</v>
+        <v>-1.7364966642881865</v>
       </c>
       <c r="U21">
-        <v>0.18462401469150699</v>
+        <v>-1.224023757981195</v>
       </c>
       <c r="V21">
-        <v>3.0468084295907166E-2</v>
+        <v>-0.24823803481894732</v>
       </c>
       <c r="W21">
-        <v>-0.37218878164786429</v>
+        <v>0.30186469568673324</v>
       </c>
       <c r="X21">
-        <v>-2.68290708017207E-2</v>
+        <v>0.4866446052762553</v>
       </c>
       <c r="Y21">
-        <v>-1.1053124237835832</v>
+        <v>1.544944738288085</v>
       </c>
       <c r="Z21">
-        <v>4.1084916371791458E-2</v>
+        <v>0.80883219984872345</v>
       </c>
       <c r="AA21">
-        <v>0.69534383285897117</v>
+        <v>0.46802136700156044</v>
       </c>
       <c r="AB21">
-        <v>0.53180775926345514</v>
+        <v>0.53838974480686719</v>
       </c>
       <c r="AC21">
-        <v>-0.52805137621320064</v>
+        <v>0.45789063337947067</v>
       </c>
       <c r="AD21">
-        <v>-0.61849582633564293</v>
+        <v>-0.57805906916970329</v>
       </c>
       <c r="AE21">
-        <v>-0.55883425812934873</v>
+        <v>-9.1900988420561935E-2</v>
       </c>
       <c r="AF21">
-        <v>0.86607087348170375</v>
+        <v>0.38381768803184735</v>
       </c>
       <c r="AG21">
-        <v>-0.70265930618851868</v>
+        <v>-0.48331282985115936</v>
       </c>
       <c r="AH21">
-        <v>-0.52334636838775495</v>
+        <v>1.1684494647053416</v>
       </c>
       <c r="AI21">
-        <v>0.41521611494262145</v>
+        <v>7.5744513706223815E-2</v>
       </c>
       <c r="AJ21">
-        <v>0.59036443317929133</v>
+        <v>0.72771955576285974</v>
       </c>
       <c r="AK21">
-        <v>-1.8965039322908157</v>
+        <v>-0.58326364236869666</v>
       </c>
       <c r="AL21">
-        <v>4.9252187037200343E-2</v>
+        <v>0.64561782409865254</v>
       </c>
       <c r="AM21">
-        <v>-0.61196996669774384</v>
+        <v>2.2833819361230332</v>
       </c>
       <c r="AN21">
-        <v>-0.77034984013139596</v>
+        <v>-0.40924538541906619</v>
       </c>
       <c r="AO21">
-        <v>-0.4006044206932905</v>
+        <v>1.1502634016398083</v>
       </c>
       <c r="AP21">
-        <v>-1.4816396827930642</v>
+        <v>1.1537608908253811</v>
       </c>
       <c r="AQ21">
-        <v>0.50335126447798739</v>
+        <v>-1.0803913878974898</v>
       </c>
       <c r="AR21">
-        <v>-0.26481003642400347</v>
+        <v>1.7607865023908376E-3</v>
       </c>
       <c r="AS21">
-        <v>0.59864364731009478</v>
+        <v>-0.15564523484337717</v>
       </c>
       <c r="AT21">
-        <v>0.78864857463271143</v>
+        <v>-0.95837332135372788</v>
       </c>
       <c r="AU21">
-        <v>-1.5120302563481118</v>
+        <v>0.13709090158339693</v>
       </c>
       <c r="AV21">
-        <v>0.6824941290487645</v>
+        <v>1.0078819464020685</v>
       </c>
       <c r="AW21">
-        <v>1.3478801667830316</v>
+        <v>-0.88837170660803466</v>
       </c>
       <c r="AX21">
-        <v>-0.6705697276385052</v>
+        <v>0.68616506224624929</v>
       </c>
       <c r="AY21">
-        <v>0.67639588334553569</v>
+        <v>1.7043268596557559</v>
       </c>
       <c r="AZ21">
-        <v>1.3135142737883081</v>
+        <v>-0.66803590135555702</v>
       </c>
       <c r="BA21">
-        <v>2.7530611938643537</v>
+        <v>-0.33896794753041987</v>
       </c>
       <c r="BB21">
-        <v>-1.1288802923744146</v>
+        <v>1.7651139471346271</v>
       </c>
     </row>
     <row r="22" spans="2:55" x14ac:dyDescent="0.3">
@@ -1225,154 +1225,154 @@
       </c>
       <c r="E23" s="5" cm="1">
         <f t="array" ref="E23:BB23">TRANSPOSE(_xll.RScript.Evaluate($B$19&amp;"$"&amp;D23))</f>
-        <v>9.8595139996497966E-2</v>
+        <v>5.3186912053523328E-2</v>
       </c>
       <c r="F23" s="5">
-        <v>9.967615769743321E-2</v>
+        <v>-0.13071696823549606</v>
       </c>
       <c r="G23" s="5">
-        <v>4.9432457647497041E-2</v>
+        <v>0.16756449756553116</v>
       </c>
       <c r="H23" s="5">
-        <v>-3.2031342812206098E-2</v>
+        <v>-1.8493442984594877E-2</v>
       </c>
       <c r="I23" s="5">
-        <v>0.1195678761251423</v>
+        <v>-1.0151098116806867E-2</v>
       </c>
       <c r="J23" s="5">
-        <v>-1.3933407767941913E-2</v>
+        <v>-0.18812705018165249</v>
       </c>
       <c r="K23" s="5">
-        <v>0.14285838121411709</v>
+        <v>0.31450157502930604</v>
       </c>
       <c r="L23" s="5">
-        <v>3.7542380260337849E-2</v>
+        <v>8.7416720058506314E-3</v>
       </c>
       <c r="M23" s="5">
-        <v>8.1389416085553612E-2</v>
+        <v>-0.17506297895860001</v>
       </c>
       <c r="N23" s="5">
-        <v>0.17410259746741352</v>
+        <v>-0.2037555103639398</v>
       </c>
       <c r="O23" s="5">
-        <v>-2.0257439088112505E-2</v>
+        <v>0.17833775270150931</v>
       </c>
       <c r="P23" s="5">
-        <v>-1.1170148780997868E-3</v>
+        <v>1.570678284235618E-2</v>
       </c>
       <c r="Q23" s="5">
-        <v>0.26465870406111247</v>
+        <v>-6.7185792331453276E-2</v>
       </c>
       <c r="R23">
-        <v>0.17249135835129709</v>
+        <v>-7.818551482944841E-2</v>
       </c>
       <c r="S23">
-        <v>9.0021786033620987E-2</v>
+        <v>0.12174193245301873</v>
       </c>
       <c r="T23">
-        <v>0.18319825281976421</v>
+        <v>0.14380074324820069</v>
       </c>
       <c r="U23">
-        <v>8.550675279214015E-2</v>
+        <v>-6.9666585972889106E-2</v>
       </c>
       <c r="V23">
-        <v>0.13871345109289956</v>
+        <v>-0.11812133585497708</v>
       </c>
       <c r="W23">
-        <v>-2.014394056981561E-3</v>
+        <v>0.17991161189476257</v>
       </c>
       <c r="X23">
-        <v>1.4100177663179475E-2</v>
+        <v>5.3661398171098718E-3</v>
       </c>
       <c r="Y23">
-        <v>0.14727880954270156</v>
+        <v>-0.12210696469467952</v>
       </c>
       <c r="Z23">
-        <v>0.26912609875475391</v>
+        <v>-0.15356589447255992</v>
       </c>
       <c r="AA23">
-        <v>0.16615032485986281</v>
+        <v>-0.13588198368541513</v>
       </c>
       <c r="AB23">
-        <v>0.21947269784490431</v>
+        <v>-2.2013515565276753E-3</v>
       </c>
       <c r="AC23">
-        <v>0.12419926525226738</v>
+        <v>-3.8400368446185523E-2</v>
       </c>
       <c r="AD23">
-        <v>6.6161999790227743E-2</v>
+        <v>-7.892500430947369E-2</v>
       </c>
       <c r="AE23">
-        <v>0.23259630326332281</v>
+        <v>-0.11348834813918218</v>
       </c>
       <c r="AF23">
-        <v>8.5581240636035338E-2</v>
+        <v>-0.15567322113814697</v>
       </c>
       <c r="AG23">
-        <v>0.18029501487448152</v>
+        <v>-0.2285832275439742</v>
       </c>
       <c r="AH23">
-        <v>0.3305489610599503</v>
+        <v>-9.4856480984296665E-3</v>
       </c>
       <c r="AI23">
-        <v>-3.575661187920548E-3</v>
+        <v>9.2576346393086831E-2</v>
       </c>
       <c r="AJ23">
-        <v>9.6110783041547077E-2</v>
+        <v>-0.34253808624395132</v>
       </c>
       <c r="AK23">
-        <v>3.084857044936351E-2</v>
+        <v>-0.18798184318148659</v>
       </c>
       <c r="AL23">
-        <v>0.12318871518330804</v>
+        <v>7.0364748980612513E-2</v>
       </c>
       <c r="AM23">
-        <v>0.16457381094881601</v>
+        <v>-0.11970957500325818</v>
       </c>
       <c r="AN23">
-        <v>3.1758310586096794E-2</v>
+        <v>-0.34419090680523778</v>
       </c>
       <c r="AO23">
-        <v>9.4982876420630913E-2</v>
+        <v>-0.16257944840404148</v>
       </c>
       <c r="AP23">
-        <v>9.648001962662045E-2</v>
+        <v>-2.3331980456966717E-2</v>
       </c>
       <c r="AQ23">
-        <v>5.553764688951851E-2</v>
+        <v>6.3191264280704429E-2</v>
       </c>
       <c r="AR23">
-        <v>4.608618014529775E-3</v>
+        <v>-0.12443487175828716</v>
       </c>
       <c r="AS23">
-        <v>-0.1185205962805387</v>
+        <v>-0.263795256242494</v>
       </c>
       <c r="AT23">
-        <v>0.11478139930632347</v>
+        <v>-0.28869403303866537</v>
       </c>
       <c r="AU23">
-        <v>2.1706471661199211E-2</v>
+        <v>-3.1688102356952574E-2</v>
       </c>
       <c r="AV23">
-        <v>5.0203323397702615E-2</v>
+        <v>-0.1913163579700507</v>
       </c>
       <c r="AW23">
-        <v>-1.819296637301826E-2</v>
+        <v>6.1734819045549116E-2</v>
       </c>
       <c r="AX23">
-        <v>0.16319261933684026</v>
+        <v>0.12276707597059477</v>
       </c>
       <c r="AY23">
-        <v>7.9735323546909709E-2</v>
+        <v>-0.30952778780818546</v>
       </c>
       <c r="AZ23">
-        <v>6.2688422526765875E-2</v>
+        <v>-2.0530085691723432E-3</v>
       </c>
       <c r="BA23">
-        <v>-0.12268937042614247</v>
+        <v>-5.9718708188772229E-2</v>
       </c>
       <c r="BB23">
-        <v>0.39641903015436442</v>
+        <v>-4.0422994967676429E-2</v>
       </c>
     </row>
     <row r="24" spans="2:55" x14ac:dyDescent="0.3">
@@ -1675,154 +1675,154 @@
         <v>y</v>
       </c>
       <c r="F31" s="5">
-        <v>0.24403989288576011</v>
+        <v>-1.8189693566204739</v>
       </c>
       <c r="G31" s="5">
-        <v>1.7979058642525871</v>
+        <v>-1.6625875328555801</v>
       </c>
       <c r="H31" s="5">
-        <v>-0.27883236733474348</v>
+        <v>0.22307911922425944</v>
       </c>
       <c r="I31" s="5">
-        <v>-2.1583701451098665</v>
+        <v>0.71467636045989646</v>
       </c>
       <c r="J31" s="5">
-        <v>-0.75694953986207336</v>
+        <v>-0.17783606523311285</v>
       </c>
       <c r="K31" s="5">
-        <v>0.24925289781350282</v>
+        <v>-0.3588608571418363</v>
       </c>
       <c r="L31" s="5">
-        <v>2.4610668844094978</v>
+        <v>7.4199672982744755E-2</v>
       </c>
       <c r="M31" s="5">
-        <v>0.9250537161654605</v>
+        <v>1.3580972518869507</v>
       </c>
       <c r="N31" s="5">
-        <v>0.6854777196380043</v>
+        <v>2.2035398668307273</v>
       </c>
       <c r="O31" s="5">
-        <v>-1.6762631932858472</v>
+        <v>0.17183076285870202</v>
       </c>
       <c r="P31" s="5">
-        <v>-0.66799800381939145</v>
+        <v>1.1237707691857339</v>
       </c>
       <c r="Q31" s="5">
-        <v>-0.33011611581020683</v>
+        <v>-3.021199721868801E-2</v>
       </c>
       <c r="R31">
-        <v>0.19204093435277206</v>
+        <v>-0.57868177141481614</v>
       </c>
       <c r="S31">
-        <v>0.58806970672574421</v>
+        <v>0.39958229683172514</v>
       </c>
       <c r="T31">
-        <v>-0.60402261864740481</v>
+        <v>4.7714125564141709E-2</v>
       </c>
       <c r="U31">
-        <v>1.0561207151615573</v>
+        <v>-1.5990810780236466</v>
       </c>
       <c r="V31">
-        <v>0.26157334654476083</v>
+        <v>-1.5540364704036937</v>
       </c>
       <c r="W31">
-        <v>0.28575666301379143</v>
+        <v>-0.68435186062181019</v>
       </c>
       <c r="X31">
-        <v>-0.58859453312588172</v>
+        <v>0.51835206289856517</v>
       </c>
       <c r="Y31">
-        <v>-0.18922168716891727</v>
+        <v>0.32093066161544137</v>
       </c>
       <c r="Z31">
-        <v>-0.82131430991603416</v>
+        <v>1.1001036017789989</v>
       </c>
       <c r="AA31">
-        <v>0.73349314559250645</v>
+        <v>0.29510560869772434</v>
       </c>
       <c r="AB31">
-        <v>1.0425958590409565</v>
+        <v>-6.9828568273302121E-3</v>
       </c>
       <c r="AC31">
-        <v>1.0577867529680895</v>
+        <v>0.35610530470982982</v>
       </c>
       <c r="AD31">
-        <v>-0.32141172806868151</v>
+        <v>0.19634139458646269</v>
       </c>
       <c r="AE31">
-        <v>-0.6063866140786488</v>
+        <v>-0.92834489198990822</v>
       </c>
       <c r="AF31">
-        <v>1.1132691626223755E-2</v>
+        <v>-0.51786998515879057</v>
       </c>
       <c r="AG31">
-        <v>0.9432698751397961</v>
+        <v>-0.13452330534017243</v>
       </c>
       <c r="AH31">
-        <v>-0.30799683273386846</v>
+        <v>-1.1613044844081504</v>
       </c>
       <c r="AI31">
-        <v>0.37494020610931506</v>
+        <v>0.97021463841976174</v>
       </c>
       <c r="AJ31">
-        <v>0.19357727790999485</v>
+        <v>0.10099430504269348</v>
       </c>
       <c r="AK31">
-        <v>0.70285655999642638</v>
+        <v>-0.19979845921476705</v>
       </c>
       <c r="AL31">
-        <v>-2.0027589597627733</v>
+        <v>-1.1723506571096332</v>
       </c>
       <c r="AM31">
-        <v>0.25250465379341991</v>
+        <v>0.62223099629758094</v>
       </c>
       <c r="AN31">
-        <v>-0.27000213052466354</v>
+        <v>1.8437903513314859</v>
       </c>
       <c r="AO31">
-        <v>-0.8735555829078353</v>
+        <v>-1.3403825729689836</v>
       </c>
       <c r="AP31">
-        <v>-0.291892833239278</v>
+        <v>0.61679987840327888</v>
       </c>
       <c r="AQ31">
-        <v>-1.3679099416040572</v>
+        <v>0.9252068227100454</v>
       </c>
       <c r="AR31">
-        <v>0.47984956391294858</v>
+        <v>-1.1194859577739902</v>
       </c>
       <c r="AS31">
-        <v>-0.45901664714474083</v>
+        <v>-0.44817775597609633</v>
       </c>
       <c r="AT31">
-        <v>-8.2698602056794513E-3</v>
+        <v>-0.91074048519615147</v>
       </c>
       <c r="AU31">
-        <v>0.96372123641063412</v>
+        <v>-1.7679892935410304</v>
       </c>
       <c r="AV31">
-        <v>-1.6489279484602835</v>
+        <v>-0.10976052312315038</v>
       </c>
       <c r="AW31">
-        <v>0.64111273918811751</v>
+        <v>0.41149336200055403</v>
       </c>
       <c r="AX31">
-        <v>1.0772467617513688</v>
+        <v>-0.93065544702825997</v>
       </c>
       <c r="AY31">
-        <v>-0.33323139639097277</v>
+        <v>0.77752333685286423</v>
       </c>
       <c r="AZ31">
-        <v>0.73400042633200502</v>
+        <v>0.8490913231879933</v>
       </c>
       <c r="BA31">
-        <v>1.3139806821714328</v>
+        <v>-0.84999551558601028</v>
       </c>
       <c r="BB31">
-        <v>2.1321747080353362</v>
+        <v>-0.64719784379485279</v>
       </c>
       <c r="BC31">
-        <v>-9.8091383340707106E-3</v>
+        <v>1.4991357735848605</v>
       </c>
     </row>
     <row r="32" spans="2:55" x14ac:dyDescent="0.3">
@@ -1830,154 +1830,154 @@
         <v>x</v>
       </c>
       <c r="F32" s="5">
-        <v>0.20869344016752428</v>
+        <v>-1.295251407374048</v>
       </c>
       <c r="G32" s="5">
-        <v>0.21993943751203449</v>
+        <v>0.16507399353648308</v>
       </c>
       <c r="H32" s="5">
-        <v>-0.3027536847668747</v>
+        <v>-2.2034894127685103</v>
       </c>
       <c r="I32" s="5">
-        <v>-1.1502344270822147</v>
+        <v>-0.72605926719765601</v>
       </c>
       <c r="J32" s="5">
-        <v>0.42687611618297483</v>
+        <v>-0.79230331867955295</v>
       </c>
       <c r="K32" s="5">
-        <v>-0.96195875937291031</v>
+        <v>0.62095018713593997</v>
       </c>
       <c r="L32" s="5">
-        <v>0.66917090761572429</v>
+        <v>-3.3702725508876514</v>
       </c>
       <c r="M32" s="5">
-        <v>-0.42644803186821123</v>
+        <v>-0.94232512387649059</v>
       </c>
       <c r="N32" s="5">
-        <v>2.9699585353038991E-2</v>
+        <v>0.51721232681267781</v>
       </c>
       <c r="O32" s="5">
-        <v>0.99420940856932749</v>
+        <v>0.7450510888974764</v>
       </c>
       <c r="P32" s="5">
-        <v>-1.0277486528888009</v>
+        <v>-2.2890365915492601</v>
       </c>
       <c r="Q32" s="5">
-        <v>-0.82862780625268107</v>
+        <v>-0.99763297414436602</v>
       </c>
       <c r="R32">
-        <v>1.9362788431420086</v>
+        <v>-0.33940796615127766</v>
       </c>
       <c r="S32">
-        <v>0.97744743436153636</v>
+        <v>-0.25206247816296168</v>
       </c>
       <c r="T32">
-        <v>0.11950348905315647</v>
+        <v>-1.8396262051868364</v>
       </c>
       <c r="U32">
-        <v>1.0888329432725401</v>
+        <v>-2.0147885871194986</v>
       </c>
       <c r="V32">
-        <v>7.2532887369020985E-2</v>
+        <v>-0.31970872998881839</v>
       </c>
       <c r="W32">
-        <v>0.62605054696287576</v>
+        <v>6.5055865170214014E-2</v>
       </c>
       <c r="X32">
-        <v>-0.83796338313916929</v>
+        <v>-2.3015341340358706</v>
       </c>
       <c r="Y32">
-        <v>-0.67032095636273525</v>
+        <v>-0.91552103801890972</v>
       </c>
       <c r="Z32">
-        <v>0.71515731949585737</v>
+        <v>9.6704545035325065E-2</v>
       </c>
       <c r="AA32">
-        <v>1.9827538535124822</v>
+        <v>0.34651044455142577</v>
       </c>
       <c r="AB32">
-        <v>0.91148066458107035</v>
+        <v>0.2060878277511787</v>
       </c>
       <c r="AC32">
-        <v>1.4662017061280042</v>
+        <v>-0.85542986508266361</v>
       </c>
       <c r="AD32">
-        <v>0.47505718646521183</v>
+        <v>-0.56798435948006576</v>
       </c>
       <c r="AE32">
-        <v>-0.12871362385994017</v>
+        <v>-0.24619041461710245</v>
       </c>
       <c r="AF32">
-        <v>1.6027286395523341</v>
+        <v>2.8266703175105594E-2</v>
       </c>
       <c r="AG32">
-        <v>7.3307796136861503E-2</v>
+        <v>0.36324409178571126</v>
       </c>
       <c r="AH32">
-        <v>1.0586301018251492</v>
+        <v>0.94220052363287798</v>
       </c>
       <c r="AI32">
-        <v>2.6217455608449884</v>
+        <v>-0.79758745712918977</v>
       </c>
       <c r="AJ32">
-        <v>-0.85420549091727582</v>
+        <v>-1.6080310583697857</v>
       </c>
       <c r="AK32">
-        <v>0.18284828361360123</v>
+        <v>1.8470817825558485</v>
       </c>
       <c r="AL32">
-        <v>-0.49608478924400329</v>
+        <v>0.61979714202129099</v>
       </c>
       <c r="AM32">
-        <v>0.46454427499096668</v>
+        <v>-1.4316554438625828</v>
       </c>
       <c r="AN32">
-        <v>0.89507994214896014</v>
+        <v>7.7667594554662003E-2</v>
       </c>
       <c r="AO32">
-        <v>-0.48662061936680379</v>
+        <v>1.8602063335169305</v>
       </c>
       <c r="AP32">
-        <v>0.17111449345205379</v>
+        <v>0.41808436532967602</v>
       </c>
       <c r="AQ32">
-        <v>0.18668950994286992</v>
+        <v>-0.68763789640842754</v>
       </c>
       <c r="AR32">
-        <v>-0.23924043984573629</v>
+        <v>-1.3746929594176893</v>
       </c>
       <c r="AS32">
-        <v>-0.76906314579381829</v>
+        <v>0.11518975486669418</v>
       </c>
       <c r="AT32">
-        <v>-2.049995748282774</v>
+        <v>1.2218086528644474</v>
       </c>
       <c r="AU32">
-        <v>0.37708164422614165</v>
+        <v>1.4195223506391097</v>
       </c>
       <c r="AV32">
-        <v>-0.59119148232230845</v>
+        <v>-0.6212844456575437</v>
       </c>
       <c r="AW32">
-        <v>-0.29473424699791345</v>
+        <v>0.64627552104080599</v>
       </c>
       <c r="AX32">
-        <v>-1.0062716181911204</v>
+        <v>-1.3631277658579346</v>
       </c>
       <c r="AY32">
-        <v>0.88071118834676099</v>
+        <v>-1.8477665615291952</v>
       </c>
       <c r="AZ32">
-        <v>1.2491800243608223E-2</v>
+        <v>1.5849569311300531</v>
       </c>
       <c r="BA32">
-        <v>-0.16484979503187619</v>
+        <v>-0.85660781212837833</v>
       </c>
       <c r="BB32">
-        <v>-2.0933641620754653</v>
+        <v>-0.39870183546581439</v>
       </c>
       <c r="BC32">
-        <v>3.3070022605997496</v>
+        <v>-0.55192329061492629</v>
       </c>
     </row>
     <row r="34" spans="2:54" x14ac:dyDescent="0.3">
@@ -2011,154 +2011,154 @@
       </c>
       <c r="E36" cm="1">
         <f t="array" ref="E36:BB36">TRANSPOSE(_xll.RScript.Evaluate($B$34&amp;"$"&amp;D36))</f>
-        <v>0.14544475288926215</v>
+        <v>-1.8721562686739972</v>
       </c>
       <c r="F36">
-        <v>1.6982297065551539</v>
+        <v>-1.5318705646200841</v>
       </c>
       <c r="G36">
-        <v>-0.32826482498224052</v>
+        <v>5.551462165872828E-2</v>
       </c>
       <c r="H36">
-        <v>-2.1263388022976604</v>
+        <v>0.73316980344449134</v>
       </c>
       <c r="I36">
-        <v>-0.87651741598721566</v>
+        <v>-0.16768496711630598</v>
       </c>
       <c r="J36">
-        <v>0.26318630558144473</v>
+        <v>-0.17073380696018381</v>
       </c>
       <c r="K36">
-        <v>2.3182085031953807</v>
+        <v>-0.24030190204656127</v>
       </c>
       <c r="L36">
-        <v>0.88751133590512266</v>
+        <v>1.3493555798811001</v>
       </c>
       <c r="M36">
-        <v>0.60408830355245069</v>
+        <v>2.3786028457893273</v>
       </c>
       <c r="N36">
-        <v>-1.8503657907532607</v>
+        <v>0.37558627322264182</v>
       </c>
       <c r="O36">
-        <v>-0.64774056473127894</v>
+        <v>0.94543301648422462</v>
       </c>
       <c r="P36">
-        <v>-0.32899910093210705</v>
+        <v>-4.591878006104419E-2</v>
       </c>
       <c r="Q36">
-        <v>-7.2617769708340385E-2</v>
+        <v>-0.51149597908336286</v>
       </c>
       <c r="R36">
-        <v>0.41557834837444713</v>
+        <v>0.47776781166117355</v>
       </c>
       <c r="S36">
-        <v>-0.69404440468102579</v>
+        <v>-7.4027806888877029E-2</v>
       </c>
       <c r="T36">
-        <v>0.87292246234179305</v>
+        <v>-1.7428818212718473</v>
       </c>
       <c r="U36">
-        <v>0.17606659375262068</v>
+        <v>-1.4843698844308046</v>
       </c>
       <c r="V36">
-        <v>0.14704321192089187</v>
+        <v>-0.56623052476683311</v>
       </c>
       <c r="W36">
-        <v>-0.58658013906890016</v>
+        <v>0.3384404510038026</v>
       </c>
       <c r="X36">
-        <v>-0.20332186483209674</v>
+        <v>0.3155645217983315</v>
       </c>
       <c r="Y36">
-        <v>-0.96859311945873572</v>
+        <v>1.2222105664736784</v>
       </c>
       <c r="Z36">
-        <v>0.46436704683775254</v>
+        <v>0.44867150317028426</v>
       </c>
       <c r="AA36">
-        <v>0.87644553418109372</v>
+        <v>0.12889912685808491</v>
       </c>
       <c r="AB36">
-        <v>0.83831405512318524</v>
+        <v>0.35830665626635749</v>
       </c>
       <c r="AC36">
-        <v>-0.44561099332094889</v>
+        <v>0.23474176303264821</v>
       </c>
       <c r="AD36">
-        <v>-0.67254861386887654</v>
+        <v>-0.84941988768043453</v>
       </c>
       <c r="AE36">
-        <v>-0.22146361163709904</v>
+        <v>-0.40438163701960839</v>
       </c>
       <c r="AF36">
-        <v>0.85768863450376076</v>
+        <v>2.1149915797974539E-2</v>
       </c>
       <c r="AG36">
-        <v>-0.48829184760834998</v>
+        <v>-0.93272125686417617</v>
       </c>
       <c r="AH36">
-        <v>4.4391245049364758E-2</v>
+        <v>0.97970028651819141</v>
       </c>
       <c r="AI36">
-        <v>0.1971529390979154</v>
+        <v>8.4179586496066494E-3</v>
       </c>
       <c r="AJ36">
-        <v>0.6067457769548793</v>
+        <v>0.1427396270291843</v>
       </c>
       <c r="AK36">
-        <v>-2.0336075302121368</v>
+        <v>-0.98436881392814657</v>
       </c>
       <c r="AL36">
-        <v>0.12931593861011187</v>
+        <v>0.55186624731696843</v>
       </c>
       <c r="AM36">
-        <v>-0.43457594147347955</v>
+        <v>1.9634999263347441</v>
       </c>
       <c r="AN36">
-        <v>-0.9053138934939321</v>
+        <v>-0.99619166616374577</v>
       </c>
       <c r="AO36">
-        <v>-0.38687570965990892</v>
+        <v>0.77937932680732036</v>
       </c>
       <c r="AP36">
-        <v>-1.4643899612306777</v>
+        <v>0.94853880316701211</v>
       </c>
       <c r="AQ36">
-        <v>0.42431191702343007</v>
+        <v>-1.1826772220546946</v>
       </c>
       <c r="AR36">
-        <v>-0.46362526515927061</v>
+        <v>-0.32374288421780917</v>
       </c>
       <c r="AS36">
-        <v>0.11025073607485925</v>
+        <v>-0.64694522895365747</v>
       </c>
       <c r="AT36">
-        <v>0.84893983710431065</v>
+        <v>-1.479295260502365</v>
       </c>
       <c r="AU36">
-        <v>-1.6706344201214827</v>
+        <v>-7.8072420766197803E-2</v>
       </c>
       <c r="AV36">
-        <v>0.59090941579041489</v>
+        <v>0.60280971997060473</v>
       </c>
       <c r="AW36">
-        <v>1.0954397281243871</v>
+        <v>-0.99239026607380909</v>
       </c>
       <c r="AX36">
-        <v>-0.49642401572781303</v>
+        <v>0.65475626088226946</v>
       </c>
       <c r="AY36">
-        <v>0.65426510278509531</v>
+        <v>1.1586191109961788</v>
       </c>
       <c r="AZ36">
-        <v>1.2512922596446669</v>
+        <v>-0.84794250701683793</v>
       </c>
       <c r="BA36">
-        <v>2.2548640784614786</v>
+        <v>-0.58747913560608056</v>
       </c>
       <c r="BB36">
-        <v>-0.40622816848843513</v>
+        <v>1.5395587685525369</v>
       </c>
     </row>
     <row r="37" spans="2:54" x14ac:dyDescent="0.3">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="E39" cm="1">
         <f t="array" ref="E39">TRANSPOSE(_xll.RScript.Evaluate($B$34&amp;"$"&amp;D39))</f>
-        <v>0.97713512136322711</v>
+        <v>0.95985448663582806</v>
       </c>
       <c r="I39" s="1"/>
       <c r="R39" s="4"/>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="E41" cm="1">
         <f t="array" ref="E41">TRANSPOSE(_xll.RScript.Evaluate($B$34&amp;"$"&amp;D41))</f>
-        <v>1.0927032743304671E-2</v>
+        <v>2.2447999635102647E-2</v>
       </c>
     </row>
     <row r="42" spans="2:54" x14ac:dyDescent="0.3">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="E42" cm="1">
         <f t="array" ref="E42">TRANSPOSE(_xll.RScript.Evaluate($B$34&amp;"$"&amp;D42))</f>
-        <v>-9.6786540745430472E-3</v>
+        <v>2.0823329608340435E-3</v>
       </c>
     </row>
     <row r="43" spans="2:54" x14ac:dyDescent="0.3">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="E43" cm="1">
         <f t="array" ref="E43:G43">TRANSPOSE(_xll.RScript.Evaluate($B$34&amp;"$"&amp;D43))</f>
-        <v>0.53029209071740879</v>
+        <v>1.1022472278535773</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2249,18 +2249,18 @@
       </c>
       <c r="E44" cm="1">
         <f t="array" ref="E44:F45">TRANSPOSE(_xll.RScript.Evaluate($B$34&amp;"$"&amp;D44))</f>
-        <v>2.0641366211616771E-2</v>
+        <v>2.2473939536264319E-2</v>
       </c>
       <c r="F44">
-        <v>-3.4211779848343422E-3</v>
+        <v>6.2157120498714238E-3</v>
       </c>
     </row>
     <row r="45" spans="2:54" x14ac:dyDescent="0.3">
       <c r="E45">
-        <v>-3.4211779848343422E-3</v>
+        <v>6.2157120498714238E-3</v>
       </c>
       <c r="F45">
-        <v>1.824926008248905E-2</v>
+        <v>1.561682317638865E-2</v>
       </c>
     </row>
     <row r="47" spans="2:54" x14ac:dyDescent="0.3">
@@ -2283,7 +2283,7 @@
         <v>Min.</v>
       </c>
       <c r="F48">
-        <v>-2.1263388022976604</v>
+        <v>-1.8721562686739972</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
@@ -2294,7 +2294,7 @@
         <v>1st Qu.</v>
       </c>
       <c r="F49">
-        <v>-0.49439097369794727</v>
+        <v>-0.63207870561676327</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
@@ -2305,7 +2305,7 @@
         <v>Median</v>
       </c>
       <c r="F50">
-        <v>7.7320990562112002E-2</v>
+        <v>1.4783937223790594E-2</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
@@ -2316,7 +2316,7 @@
         <v>Mean</v>
       </c>
       <c r="F51">
-        <v>2.1103995287430344E-17</v>
+        <v>3.3315364356134577E-17</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
@@ -2327,7 +2327,7 @@
         <v>3rd Qu.</v>
       </c>
       <c r="F52">
-        <v>0.60608140860427218</v>
+        <v>0.59007385180719574</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
@@ -2338,7 +2338,7 @@
         <v>Max.</v>
       </c>
       <c r="F53">
-        <v>2.3182085031953807</v>
+        <v>2.3786028457893273</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
@@ -2372,16 +2372,16 @@
         <v>(Intercept)</v>
       </c>
       <c r="F56">
-        <v>7.85E-2</v>
+        <v>-0.1099</v>
       </c>
       <c r="G56">
-        <v>0.1404</v>
+        <v>0.1439</v>
       </c>
       <c r="H56">
-        <v>0.55940000000000001</v>
+        <v>-0.76400000000000001</v>
       </c>
       <c r="I56">
-        <v>0.57850000000000001</v>
+        <v>0.4486</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
@@ -2389,16 +2389,16 @@
         <v>x</v>
       </c>
       <c r="F57">
-        <v>9.6100000000000005E-2</v>
+        <v>-0.12590000000000001</v>
       </c>
       <c r="G57">
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="H57">
-        <v>0.72819999999999996</v>
+        <v>-1.0499000000000001</v>
       </c>
       <c r="I57">
-        <v>0.47</v>
+        <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
@@ -2433,16 +2433,16 @@
         <v>1</v>
       </c>
       <c r="G60">
-        <v>0.26452252628379735</v>
+        <v>1.0155231164606251</v>
       </c>
       <c r="H60">
-        <v>0.26452252628379735</v>
+        <v>1.0155231164606251</v>
       </c>
       <c r="I60">
-        <v>0.3670113113185195</v>
+        <v>1.1022472278535758</v>
       </c>
       <c r="J60">
-        <v>0.54749204609353308</v>
+        <v>0.29903082980342544</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
@@ -2453,10 +2453,10 @@
         <v>48</v>
       </c>
       <c r="G61">
-        <v>34.595885385676326</v>
+        <v>44.22339050471659</v>
       </c>
       <c r="H61">
-        <v>0.72074761220159012</v>
+        <v>0.92132063551492893</v>
       </c>
       <c r="I61" t="str">
         <v/>
@@ -2480,8 +2480,7 @@
       </c>
       <c r="D85" t="str" cm="1">
         <f t="array" ref="D85">_xll.RScript.Evaluate(B85)</f>
-        <v xml:space="preserve">Exception: Error: object 'fm' not found
-</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
@@ -2516,9 +2515,7 @@
       </c>
       <c r="D95" t="str" cm="1">
         <f t="array" ref="D95">_xll.RScript.Evaluate(B95, "true")</f>
-        <v xml:space="preserve">Exception: Error in ggplot(df, aes(x = x, y = y)) : 
-i Have you misspelled the `data` argument in `ggplot()`
-</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.3">
@@ -2534,7 +2531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A073C2-CAA1-4EC5-884E-E8AA37D56572}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2601,22 +2598,22 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D6" s="10">
-        <v>-2.1263388022976604</v>
+        <v>-1.8721562686739972</v>
       </c>
       <c r="E6" s="10">
-        <v>-0.49439097369794727</v>
+        <v>-0.63207870561676327</v>
       </c>
       <c r="F6" s="10">
-        <v>7.7320990562112002E-2</v>
+        <v>1.4783937223790594E-2</v>
       </c>
       <c r="G6" s="9">
-        <v>2.1103995287430344E-17</v>
+        <v>3.3315364356134577E-17</v>
       </c>
       <c r="H6" s="10">
-        <v>0.60608140860427218</v>
+        <v>0.59007385180719574</v>
       </c>
       <c r="I6" s="10">
-        <v>2.3182085031953807</v>
+        <v>2.3786028457893273</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -2647,16 +2644,16 @@
         <v>(Intercept)</v>
       </c>
       <c r="E9" s="8">
-        <v>7.85E-2</v>
+        <v>-0.1099</v>
       </c>
       <c r="F9" s="8">
-        <v>0.1404</v>
+        <v>0.1439</v>
       </c>
       <c r="G9" s="8">
-        <v>0.55940000000000001</v>
+        <v>-0.76400000000000001</v>
       </c>
       <c r="H9" s="8">
-        <v>0.57850000000000001</v>
+        <v>0.4486</v>
       </c>
       <c r="I9" s="8"/>
     </row>
@@ -2665,23 +2662,23 @@
         <v>x</v>
       </c>
       <c r="E10" s="8">
-        <v>9.6100000000000005E-2</v>
+        <v>-0.12590000000000001</v>
       </c>
       <c r="F10" s="10">
-        <v>0.13200000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="G10" s="8">
-        <v>0.72819999999999996</v>
+        <v>-1.0499000000000001</v>
       </c>
       <c r="H10" s="10">
-        <v>0.47</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="I10" s="8"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="str">
         <f>"Residual standard error: "&amp;ROUND('Linear Model'!E39, 3)&amp;" on "&amp;'Linear Model'!E26&amp;" degrees of freedom"</f>
-        <v>Residual standard error: 0.977 on 48 degrees of freedom</v>
+        <v>Residual standard error: 0.96 on 48 degrees of freedom</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -2694,11 +2691,11 @@
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="str">
         <f>"Multiple R-squared: "&amp;ROUND('Linear Model'!E41, 4)</f>
-        <v>Multiple R-squared: 0.0109</v>
+        <v>Multiple R-squared: 0.0224</v>
       </c>
       <c r="C13" s="8" t="str">
         <f>"Adjusted R-squared: "&amp;ROUND('Linear Model'!E42, 4)</f>
-        <v>Adjusted R-squared: -0.0097</v>
+        <v>Adjusted R-squared: 0.0021</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -2710,7 +2707,7 @@
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="str">
         <f>"F-statistic: "&amp;ROUND('Linear Model'!E43, 2)&amp;" on "&amp;'Linear Model'!F43&amp;" and "&amp;'Linear Model'!G43&amp;" DF"</f>
-        <v>F-statistic: 0.53 on 1 and 48 DF</v>
+        <v>F-statistic: 1.1 on 1 and 48 DF</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -2755,16 +2752,16 @@
         <v>1</v>
       </c>
       <c r="F17" s="10">
-        <v>0.26452252628379735</v>
+        <v>1.0155231164606251</v>
       </c>
       <c r="G17" s="10">
-        <v>0.26452252628379735</v>
+        <v>1.0155231164606251</v>
       </c>
       <c r="H17" s="10">
-        <v>0.3670113113185195</v>
+        <v>1.1022472278535758</v>
       </c>
       <c r="I17" s="10">
-        <v>0.54749204609353308</v>
+        <v>0.29903082980342544</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
@@ -2777,10 +2774,10 @@
         <v>48</v>
       </c>
       <c r="F18" s="10">
-        <v>34.595885385676326</v>
+        <v>44.22339050471659</v>
       </c>
       <c r="G18" s="10">
-        <v>0.72074761220159012</v>
+        <v>0.92132063551492893</v>
       </c>
       <c r="H18" s="8" t="str">
         <v/>
@@ -2801,8 +2798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E54137A-AC86-4C17-97C8-77A96C22EEAE}">
   <dimension ref="B2:Q57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2834,49 +2831,49 @@
       </c>
       <c r="C4" cm="1">
         <f t="array" ref="C4:Q4">TRANSPOSE(_xll.RScript.Evaluate(B4))</f>
-        <v>-1.4962089497519335</v>
+        <v>0.6825695723586126</v>
       </c>
       <c r="D4">
-        <v>-3.3915554526448028</v>
+        <v>-0.31391240127077941</v>
       </c>
       <c r="E4">
-        <v>0.67773592231112656</v>
+        <v>-1.5138772408458816</v>
       </c>
       <c r="F4">
-        <v>1.5552069819211933</v>
+        <v>1.1290175656535473</v>
       </c>
       <c r="G4">
-        <v>-1.2253252148789326</v>
+        <v>-0.78737788383067109</v>
       </c>
       <c r="H4">
-        <v>-0.95192824683587396</v>
+        <v>-0.63378317597523526</v>
       </c>
       <c r="I4">
-        <v>-0.84677764343094009</v>
+        <v>-4.8377400460099473E-2</v>
       </c>
       <c r="J4">
-        <v>-0.97594908106725586</v>
+        <v>-9.7205911744182028E-2</v>
       </c>
       <c r="K4">
-        <v>2.2907480314435764</v>
+        <v>1.4992888816062897</v>
       </c>
       <c r="L4">
-        <v>-1.6423544299200215</v>
+        <v>-0.69248746941944561</v>
       </c>
       <c r="M4">
-        <v>-2.0242010386831493</v>
+        <v>2.7839338190223062</v>
       </c>
       <c r="N4">
-        <v>-1.0441075648736</v>
+        <v>-1.9564084107567572</v>
       </c>
       <c r="O4">
-        <v>1.4814564492607833</v>
+        <v>1.0051991731802767</v>
       </c>
       <c r="P4">
-        <v>0.67805394991365231</v>
+        <v>0.59090383376798983</v>
       </c>
       <c r="Q4">
-        <v>0.33821709346702805</v>
+        <v>1.9228026286821878</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
@@ -2893,10 +2890,17 @@
         <v>10</v>
       </c>
       <c r="C6" t="str" cm="1">
-        <f t="array" ref="C6">TRANSPOSE(_xll.RScript.Evaluate(B6))</f>
-        <v xml:space="preserve">Exception: Error in model.frame.default(Terms, newdata, na.action = na.action, xlev = object$xlevels) : 
-  'data' must be a data.frame, environment, or list
-</v>
+        <f t="array" ref="C6:F6">TRANSPOSE(_xll.RScript.Evaluate(B6))</f>
+        <v>fit</v>
+      </c>
+      <c r="D6" t="str">
+        <v>se.fit</v>
+      </c>
+      <c r="E6" t="str">
+        <v>df</v>
+      </c>
+      <c r="F6" t="str">
+        <v>residual.scale</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -2905,9 +2909,7 @@
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">TRANSPOSE(_xll.RScript.Evaluate(B7))</f>
-        <v xml:space="preserve">Exception: Error in model.frame.default(Terms, newdata, na.action = na.action, xlev = object$xlevels) : 
-  'data' must be a data.frame, environment, or list
-</v>
+        <v>pred.w.plim</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -2916,9 +2918,7 @@
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" ref="C8">TRANSPOSE(_xll.RScript.Evaluate(B8))</f>
-        <v xml:space="preserve">Exception: Error in model.frame.default(Terms, newdata, na.action = na.action, xlev = object$xlevels) : 
-  'data' must be a data.frame, environment, or list
-</v>
+        <v>pred.w.clim</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -2927,8 +2927,7 @@
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">TRANSPOSE(_xll.RScript.Evaluate(B9))</f>
-        <v xml:space="preserve">Exception: Error: object 'pred.w.clim' not found
-</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
@@ -2965,8 +2964,7 @@
       </c>
       <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">TRANSPOSE(_xll.RScript.Evaluate(B29))</f>
-        <v xml:space="preserve">Exception: Error in eval(extras, data, env) : object 'w' not found
-</v>
+        <v>wfit</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
@@ -2975,191 +2973,677 @@
       </c>
       <c r="C30" cm="1">
         <f t="array" ref="C30:Q32">TRANSPOSE(_xll.RScript.Evaluate(B30))</f>
-        <v>-1.4962089497519335</v>
+        <v>0.6825695723586126</v>
       </c>
       <c r="D30">
-        <v>-3.3915554526448028</v>
+        <v>-0.31391240127077941</v>
       </c>
       <c r="E30">
-        <v>0.67773592231112656</v>
+        <v>-1.5138772408458816</v>
       </c>
       <c r="F30">
-        <v>1.5552069819211933</v>
+        <v>1.1290175656535473</v>
       </c>
       <c r="G30">
-        <v>-1.2253252148789326</v>
+        <v>-0.78737788383067109</v>
       </c>
       <c r="H30">
-        <v>-0.95192824683587396</v>
+        <v>-0.63378317597523526</v>
       </c>
       <c r="I30">
-        <v>-0.84677764343094009</v>
+        <v>-4.8377400460099473E-2</v>
       </c>
       <c r="J30">
-        <v>-0.97594908106725586</v>
+        <v>-9.7205911744182028E-2</v>
       </c>
       <c r="K30">
-        <v>2.2907480314435764</v>
+        <v>1.4992888816062897</v>
       </c>
       <c r="L30">
-        <v>-1.6423544299200215</v>
+        <v>-0.69248746941944561</v>
       </c>
       <c r="M30">
-        <v>-2.0242010386831493</v>
+        <v>2.7839338190223062</v>
       </c>
       <c r="N30">
-        <v>-1.0441075648736</v>
+        <v>-1.9564084107567572</v>
       </c>
       <c r="O30">
-        <v>1.4814564492607833</v>
+        <v>1.0051991731802767</v>
       </c>
       <c r="P30">
-        <v>0.67805394991365231</v>
+        <v>0.59090383376798983</v>
       </c>
       <c r="Q30">
-        <v>0.33821709346702805</v>
+        <v>1.9228026286821878</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C31">
-        <v>-4.2502440700749835</v>
+        <v>-1.9119735489604932</v>
       </c>
       <c r="D31">
-        <v>-6.4147440359458834</v>
+        <v>-2.9139035446745973</v>
       </c>
       <c r="E31">
-        <v>-2.0810146552176167</v>
+        <v>-4.2508656638733493</v>
       </c>
       <c r="F31">
-        <v>-1.3029185344471994</v>
+        <v>-1.4957394988907478</v>
       </c>
       <c r="G31">
-        <v>-3.9607414902453839</v>
+        <v>-3.4250792760345967</v>
       </c>
       <c r="H31">
-        <v>-3.6740201708791056</v>
+        <v>-3.2568348179746112</v>
       </c>
       <c r="I31">
-        <v>-3.565225467809567</v>
+        <v>-2.6370217939997831</v>
       </c>
       <c r="J31">
-        <v>-3.6989893271417484</v>
+        <v>-2.6874003920094589</v>
       </c>
       <c r="K31">
-        <v>-0.68909380424313893</v>
+        <v>-1.1653157846007915</v>
       </c>
       <c r="L31">
-        <v>-4.4086368172068973</v>
+        <v>-3.3208676765595371</v>
       </c>
       <c r="M31">
-        <v>-4.8295895790485339</v>
+        <v>-0.11324524920646484</v>
       </c>
       <c r="N31">
-        <v>-3.7700725850873864</v>
+        <v>-4.7765115611209943</v>
       </c>
       <c r="O31">
-        <v>-1.3663221106124519</v>
+        <v>-1.6091934801105376</v>
       </c>
       <c r="P31">
-        <v>-2.0807229515572621</v>
+        <v>-1.9999109713501353</v>
       </c>
       <c r="Q31">
-        <v>-2.3966042238742369</v>
+        <v>-0.80301930743650884</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C32">
-        <v>1.2578261705711162</v>
+        <v>3.2771126936777182</v>
       </c>
       <c r="D32">
-        <v>-0.36836686934372187</v>
+        <v>2.2860787421330384</v>
       </c>
       <c r="E32">
-        <v>3.4364864998398703</v>
+        <v>1.2231111821815859</v>
       </c>
       <c r="F32">
-        <v>4.4133324982895861</v>
+        <v>3.7537746301978423</v>
       </c>
       <c r="G32">
-        <v>1.5100910604875186</v>
+        <v>1.8503235083732545</v>
       </c>
       <c r="H32">
-        <v>1.7701636772073575</v>
+        <v>1.9892684660241409</v>
       </c>
       <c r="I32">
-        <v>1.871670180947687</v>
+        <v>2.5402669930795838</v>
       </c>
       <c r="J32">
-        <v>1.7470911650072365</v>
+        <v>2.4929885685210946</v>
       </c>
       <c r="K32">
-        <v>5.2705898671302922</v>
+        <v>4.1638935478133714</v>
       </c>
       <c r="L32">
-        <v>1.1239279573668539</v>
+        <v>1.9358927377206461</v>
       </c>
       <c r="M32">
-        <v>0.78118750168223583</v>
+        <v>5.6811128872510768</v>
       </c>
       <c r="N32">
-        <v>1.6818574553401862</v>
+        <v>0.86369473960747944</v>
       </c>
       <c r="O32">
-        <v>4.3292350091340186</v>
+        <v>3.6195918264710913</v>
       </c>
       <c r="P32">
-        <v>3.4368308513845669</v>
+        <v>3.1817186388861147</v>
       </c>
       <c r="Q32">
-        <v>3.0730384108082931</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+        <v>4.6486245648008842</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>20</v>
       </c>
-      <c r="C34" t="str" cm="1">
-        <f t="array" ref="C34">TRANSPOSE(_xll.RScript.Evaluate(B34))</f>
-        <v xml:space="preserve">Exception: Error: object 'wfit' not found
-</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C34" cm="1">
+        <f t="array" ref="C34:Q36">TRANSPOSE(_xll.RScript.Evaluate(B34))</f>
+        <v>0.53134654951377946</v>
+      </c>
+      <c r="D34">
+        <v>-0.27098891219248866</v>
+      </c>
+      <c r="E34">
+        <v>-1.2371622791678647</v>
+      </c>
+      <c r="F34">
+        <v>0.89081221603606142</v>
+      </c>
+      <c r="G34">
+        <v>-0.65220819824547915</v>
+      </c>
+      <c r="H34">
+        <v>-0.52853864465186506</v>
+      </c>
+      <c r="I34">
+        <v>-5.7188609615367203E-2</v>
+      </c>
+      <c r="J34">
+        <v>-9.6503767523195672E-2</v>
+      </c>
+      <c r="K34">
+        <v>1.1889428547263912</v>
+      </c>
+      <c r="L34">
+        <v>-0.57580546696391433</v>
+      </c>
+      <c r="M34">
+        <v>2.223297932155659</v>
+      </c>
+      <c r="N34">
+        <v>-1.5934742445882342</v>
+      </c>
+      <c r="O34">
+        <v>0.79111760065738201</v>
+      </c>
+      <c r="P34">
+        <v>0.45754022422032609</v>
+      </c>
+      <c r="Q34">
+        <v>1.5299425986168607</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>-2.9428481507613573</v>
+      </c>
+      <c r="D35">
+        <v>-3.7230334866676351</v>
+      </c>
+      <c r="E35">
+        <v>-3.4695020141055393</v>
+      </c>
+      <c r="F35">
+        <v>-2.0352765707634028</v>
+      </c>
+      <c r="G35">
+        <v>-3.5347139652695887</v>
+      </c>
+      <c r="H35">
+        <v>-3.5938573304888211</v>
+      </c>
+      <c r="I35">
+        <v>-3.7588858218894226</v>
+      </c>
+      <c r="J35">
+        <v>-3.7620243866963516</v>
+      </c>
+      <c r="K35">
+        <v>-1.3296492032096874</v>
+      </c>
+      <c r="L35">
+        <v>-3.57007212646237</v>
+      </c>
+      <c r="M35">
+        <v>0.40163210340474609</v>
+      </c>
+      <c r="N35">
+        <v>-3.6116693758858873</v>
+      </c>
+      <c r="O35">
+        <v>-2.2879850142211442</v>
+      </c>
+      <c r="P35">
+        <v>-3.1143006295551583</v>
+      </c>
+      <c r="Q35">
+        <v>-0.64385712111847182</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>4.0055412497889158</v>
+      </c>
+      <c r="D36">
+        <v>3.1810556622826578</v>
+      </c>
+      <c r="E36">
+        <v>0.99517745576980965</v>
+      </c>
+      <c r="F36">
+        <v>3.8169010028355257</v>
+      </c>
+      <c r="G36">
+        <v>2.2302975687786306</v>
+      </c>
+      <c r="H36">
+        <v>2.5367800411850912</v>
+      </c>
+      <c r="I36">
+        <v>3.6445086026586884</v>
+      </c>
+      <c r="J36">
+        <v>3.5690168516499607</v>
+      </c>
+      <c r="K36">
+        <v>3.7075349126624699</v>
+      </c>
+      <c r="L36">
+        <v>2.4184611925345418</v>
+      </c>
+      <c r="M36">
+        <v>4.0449637609065716</v>
+      </c>
+      <c r="N36">
+        <v>0.42472088670941899</v>
+      </c>
+      <c r="O36">
+        <v>3.870220215535908</v>
+      </c>
+      <c r="P36">
+        <v>4.0293810779958106</v>
+      </c>
+      <c r="Q36">
+        <v>3.7037423183521931</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>21</v>
       </c>
-      <c r="C39" t="str" cm="1">
-        <f t="array" ref="C39">TRANSPOSE(_xll.RScript.Evaluate(B39))</f>
-        <v xml:space="preserve">Exception: Error: object 'wfit' not found
-</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C39" cm="1">
+        <f t="array" ref="C39:O41">TRANSPOSE(_xll.RScript.Evaluate(B39))</f>
+        <v>-2.5014347554174909</v>
+      </c>
+      <c r="D39">
+        <v>-2.0609613559612114</v>
+      </c>
+      <c r="E39">
+        <v>-1.6204879565049317</v>
+      </c>
+      <c r="F39">
+        <v>-1.1800145570486522</v>
+      </c>
+      <c r="G39">
+        <v>-0.73954115759237249</v>
+      </c>
+      <c r="H39">
+        <v>-0.29906775813609288</v>
+      </c>
+      <c r="I39">
+        <v>0.14140564132018674</v>
+      </c>
+      <c r="J39">
+        <v>0.58187904077646635</v>
+      </c>
+      <c r="K39">
+        <v>1.022352440232746</v>
+      </c>
+      <c r="L39">
+        <v>1.4628258396890257</v>
+      </c>
+      <c r="M39">
+        <v>1.9032992391453052</v>
+      </c>
+      <c r="N39">
+        <v>2.3437726386015845</v>
+      </c>
+      <c r="O39">
+        <v>2.7842460380578649</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>-6.5155088272457258</v>
+      </c>
+      <c r="D40">
+        <v>-6.0112003684853033</v>
+      </c>
+      <c r="E40">
+        <v>-5.5168932559656438</v>
+      </c>
+      <c r="F40">
+        <v>-5.0330067266381961</v>
+      </c>
+      <c r="G40">
+        <v>-4.5598960442260417</v>
+      </c>
+      <c r="H40">
+        <v>-4.0978389621424345</v>
+      </c>
+      <c r="I40">
+        <v>-3.647024410905197</v>
+      </c>
+      <c r="J40">
+        <v>-3.2075444325866878</v>
+      </c>
+      <c r="K40">
+        <v>-2.7793901417948064</v>
+      </c>
+      <c r="L40">
+        <v>-2.3624521187320315</v>
+      </c>
+      <c r="M40">
+        <v>-1.9565251944289785</v>
+      </c>
+      <c r="N40">
+        <v>-1.5613171499316718</v>
+      </c>
+      <c r="O40">
+        <v>-1.1764604967223864</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>1.5126393164107439</v>
+      </c>
+      <c r="D41">
+        <v>1.8892776565628804</v>
+      </c>
+      <c r="E41">
+        <v>2.2759173429557809</v>
+      </c>
+      <c r="F41">
+        <v>2.6729776125408913</v>
+      </c>
+      <c r="G41">
+        <v>3.0808137290412971</v>
+      </c>
+      <c r="H41">
+        <v>3.4997034458702485</v>
+      </c>
+      <c r="I41">
+        <v>3.9298356935455709</v>
+      </c>
+      <c r="J41">
+        <v>4.3713025141396207</v>
+      </c>
+      <c r="K41">
+        <v>4.8240950222602983</v>
+      </c>
+      <c r="L41">
+        <v>5.2881037981100834</v>
+      </c>
+      <c r="M41">
+        <v>5.7631236727195887</v>
+      </c>
+      <c r="N41">
+        <v>6.2488624271348403</v>
+      </c>
+      <c r="O41">
+        <v>6.7449525728381161</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>22</v>
       </c>
-      <c r="C43" t="str" cm="1">
-        <f t="array" ref="C43">TRANSPOSE(_xll.RScript.Evaluate(B43))</f>
-        <v xml:space="preserve">Exception: Error: object 'wfit' not found
-</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C43" cm="1">
+        <f t="array" ref="C43:O45">TRANSPOSE(_xll.RScript.Evaluate(B43))</f>
+        <v>-2.5014347554174909</v>
+      </c>
+      <c r="D43">
+        <v>-2.0609613559612114</v>
+      </c>
+      <c r="E43">
+        <v>-1.6204879565049317</v>
+      </c>
+      <c r="F43">
+        <v>-1.1800145570486522</v>
+      </c>
+      <c r="G43">
+        <v>-0.73954115759237249</v>
+      </c>
+      <c r="H43">
+        <v>-0.29906775813609288</v>
+      </c>
+      <c r="I43">
+        <v>0.14140564132018674</v>
+      </c>
+      <c r="J43">
+        <v>0.58187904077646635</v>
+      </c>
+      <c r="K43">
+        <v>1.022352440232746</v>
+      </c>
+      <c r="L43">
+        <v>1.4628258396890257</v>
+      </c>
+      <c r="M43">
+        <v>1.9032992391453052</v>
+      </c>
+      <c r="N43">
+        <v>2.3437726386015845</v>
+      </c>
+      <c r="O43">
+        <v>2.7842460380578649</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>-4.4296385147494908</v>
+      </c>
+      <c r="D44">
+        <v>-4.0335947455853072</v>
+      </c>
+      <c r="E44">
+        <v>-3.793928572041966</v>
+      </c>
+      <c r="F44">
+        <v>-3.8443691854774213</v>
+      </c>
+      <c r="G44">
+        <v>-4.5598960442260417</v>
+      </c>
+      <c r="H44">
+        <v>-7.7999465902454261</v>
+      </c>
+      <c r="I44" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J44">
+        <v>-6.9142700275167819</v>
+      </c>
+      <c r="K44">
+        <v>-2.7793901417948064</v>
+      </c>
+      <c r="L44">
+        <v>-1.1612908471778989</v>
+      </c>
+      <c r="M44">
+        <v>-0.20385868317981548</v>
+      </c>
+      <c r="N44">
+        <v>0.46318217539614537</v>
+      </c>
+      <c r="O44">
+        <v>0.96975565835635358</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>-0.57323099608549111</v>
+      </c>
+      <c r="D45">
+        <v>-8.8327966337115482E-2</v>
+      </c>
+      <c r="E45">
+        <v>0.55295265903210233</v>
+      </c>
+      <c r="F45">
+        <v>1.4843400713801171</v>
+      </c>
+      <c r="G45">
+        <v>3.0808137290412971</v>
+      </c>
+      <c r="H45">
+        <v>7.2018110739732411</v>
+      </c>
+      <c r="I45" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J45">
+        <v>8.0780281090697148</v>
+      </c>
+      <c r="K45">
+        <v>4.8240950222602983</v>
+      </c>
+      <c r="L45">
+        <v>4.0869425265559505</v>
+      </c>
+      <c r="M45">
+        <v>4.0104571614704261</v>
+      </c>
+      <c r="N45">
+        <v>4.2243631018070236</v>
+      </c>
+      <c r="O45">
+        <v>4.5987364177593761</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>23</v>
       </c>
-      <c r="C48" t="str" cm="1">
-        <f t="array" ref="C48">TRANSPOSE(_xll.RScript.Evaluate(B48))</f>
-        <v xml:space="preserve">Exception: Error: object 'wfit' not found
-</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C48" cm="1">
+        <f t="array" ref="C48:O50">TRANSPOSE(_xll.RScript.Evaluate(B48))</f>
+        <v>-2.5014347554174909</v>
+      </c>
+      <c r="D48">
+        <v>-2.0609613559612114</v>
+      </c>
+      <c r="E48">
+        <v>-1.6204879565049317</v>
+      </c>
+      <c r="F48">
+        <v>-1.1800145570486522</v>
+      </c>
+      <c r="G48">
+        <v>-0.73954115759237249</v>
+      </c>
+      <c r="H48">
+        <v>-0.29906775813609288</v>
+      </c>
+      <c r="I48">
+        <v>0.14140564132018674</v>
+      </c>
+      <c r="J48">
+        <v>0.58187904077646635</v>
+      </c>
+      <c r="K48">
+        <v>1.022352440232746</v>
+      </c>
+      <c r="L48">
+        <v>1.4628258396890257</v>
+      </c>
+      <c r="M48">
+        <v>1.9032992391453052</v>
+      </c>
+      <c r="N48">
+        <v>2.3437726386015845</v>
+      </c>
+      <c r="O48">
+        <v>2.7842460380578649</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>-4.4296385147494908</v>
+      </c>
+      <c r="D49">
+        <v>-4.0335947455853072</v>
+      </c>
+      <c r="E49">
+        <v>-3.793928572041966</v>
+      </c>
+      <c r="F49">
+        <v>-3.8443691854774213</v>
+      </c>
+      <c r="G49">
+        <v>-4.5598960442260417</v>
+      </c>
+      <c r="H49">
+        <v>-7.7999465902454261</v>
+      </c>
+      <c r="I49" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J49">
+        <v>-6.9142700275167819</v>
+      </c>
+      <c r="K49">
+        <v>-2.7793901417948064</v>
+      </c>
+      <c r="L49">
+        <v>-1.1612908471778989</v>
+      </c>
+      <c r="M49">
+        <v>-0.20385868317981548</v>
+      </c>
+      <c r="N49">
+        <v>0.46318217539614537</v>
+      </c>
+      <c r="O49">
+        <v>0.96975565835635358</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>-0.57323099608549111</v>
+      </c>
+      <c r="D50">
+        <v>-8.8327966337115482E-2</v>
+      </c>
+      <c r="E50">
+        <v>0.55295265903210233</v>
+      </c>
+      <c r="F50">
+        <v>1.4843400713801171</v>
+      </c>
+      <c r="G50">
+        <v>3.0808137290412971</v>
+      </c>
+      <c r="H50">
+        <v>7.2018110739732411</v>
+      </c>
+      <c r="I50" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="J50">
+        <v>8.0780281090697148</v>
+      </c>
+      <c r="K50">
+        <v>4.8240950222602983</v>
+      </c>
+      <c r="L50">
+        <v>4.0869425265559505</v>
+      </c>
+      <c r="M50">
+        <v>4.0104571614704261</v>
+      </c>
+      <c r="N50">
+        <v>4.2243631018070236</v>
+      </c>
+      <c r="O50">
+        <v>4.5987364177593761</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>25</v>
       </c>
@@ -3168,44 +3652,40 @@
         <v>npk.aov</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>28</v>
       </c>
       <c r="C54" t="str" cm="1">
         <f t="array" ref="C54">TRANSPOSE(_xll.RScript.Evaluate(B54))</f>
-        <v xml:space="preserve">Exception: Error: object 'npk.aov' not found
-</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+        <v>termL</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>29</v>
       </c>
       <c r="C55" t="str" cm="1">
         <f t="array" ref="C55">TRANSPOSE(_xll.RScript.Evaluate(B55))</f>
-        <v xml:space="preserve">Exception: Error: object 'npk.aov' not found
-</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+        <v>pt</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>26</v>
       </c>
       <c r="C56" t="str" cm="1">
         <f t="array" ref="C56">TRANSPOSE(_xll.RScript.Evaluate(B56))</f>
-        <v xml:space="preserve">Exception: Error: object 'npk.aov' not found
-</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+        <v>pt.</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>27</v>
       </c>
       <c r="C57" t="str" cm="1">
         <f t="array" ref="C57">TRANSPOSE(_xll.RScript.Evaluate(B57))</f>
-        <v xml:space="preserve">Exception: Error in pt[, 1:4] : object of type 'closure' is not subsettable
-</v>
+        <v>OK</v>
       </c>
     </row>
   </sheetData>

</xml_diff>